<commit_message>
add updated 2020 data
</commit_message>
<xml_diff>
--- a/data/Data for web team 2020 v6 CORRECTED.xlsx
+++ b/data/Data for web team 2020 v6 CORRECTED.xlsx
@@ -16461,23 +16461,39 @@
       <c r="M4" s="7"/>
     </row>
     <row r="5" ht="15" customHeight="1">
-      <c r="A5" t="s" s="5">
+      <c r="A5" t="s" s="53">
         <v>16</v>
       </c>
-      <c r="B5" t="s" s="5">
+      <c r="B5" t="s" s="53">
         <v>17</v>
       </c>
-      <c r="C5" s="6"/>
-      <c r="D5" s="6"/>
-      <c r="E5" s="6"/>
-      <c r="F5" s="6"/>
-      <c r="G5" s="6"/>
-      <c r="H5" s="6"/>
-      <c r="I5" s="6"/>
-      <c r="J5" s="6"/>
-      <c r="K5" s="7"/>
-      <c r="L5" s="7"/>
-      <c r="M5" s="7"/>
+      <c r="C5" s="54">
+        <v>41937</v>
+      </c>
+      <c r="D5" s="54">
+        <v>10080</v>
+      </c>
+      <c r="E5" s="54">
+        <v>8339</v>
+      </c>
+      <c r="F5" s="54">
+        <v>5335</v>
+      </c>
+      <c r="G5" s="54">
+        <v>3004</v>
+      </c>
+      <c r="H5" s="54">
+        <v>1741</v>
+      </c>
+      <c r="I5" s="54">
+        <v>566</v>
+      </c>
+      <c r="J5" s="54">
+        <v>1175</v>
+      </c>
+      <c r="K5" s="56"/>
+      <c r="L5" s="56"/>
+      <c r="M5" s="56"/>
     </row>
     <row r="6" ht="15" customHeight="1">
       <c r="A6" t="s" s="5">
@@ -17847,35 +17863,35 @@
       </c>
       <c r="C53" s="10">
         <f>SUM(C2:C51)</f>
-        <v>967171</v>
+        <v>1009108</v>
       </c>
       <c r="D53" s="10">
         <f>SUM(D2:D51)</f>
-        <v>218008</v>
+        <v>228088</v>
       </c>
       <c r="E53" s="10">
         <f>SUM(E2:E51)</f>
-        <v>109850</v>
+        <v>118189</v>
       </c>
       <c r="F53" s="10">
         <f>SUM(F2:F51)+E9+E20+E21+E29+E30+E41+E44+E45+E47</f>
-        <v>80073</v>
+        <v>85408</v>
       </c>
       <c r="G53" s="10">
         <f>SUM(G2:G51)</f>
-        <v>29777</v>
+        <v>32781</v>
       </c>
       <c r="H53" s="10">
         <f>SUM(H2:H51)</f>
-        <v>108158</v>
+        <v>109899</v>
       </c>
       <c r="I53" s="10">
         <f>SUM(I2:I51)+H21+H29+H41+H45+H47</f>
-        <v>76152</v>
+        <v>76718</v>
       </c>
       <c r="J53" s="10">
         <f>SUM(J2:J51)</f>
-        <v>32006</v>
+        <v>33181</v>
       </c>
       <c r="K53" s="7"/>
       <c r="L53" s="6"/>
@@ -17903,35 +17919,35 @@
       </c>
       <c r="C55" s="8">
         <f>COUNTIF(C2:C51,"&gt;0")</f>
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D55" s="8">
         <f>COUNTIF(D2:D51,"&gt;0")</f>
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E55" s="8">
         <f>COUNTIF(E2:E51,"&gt;0")</f>
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="F55" s="8">
         <f>COUNTIF(F2:F51,"&gt;0")</f>
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="G55" s="8">
         <f>COUNTIF(G2:G51,"&gt;0")</f>
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="H55" s="8">
         <f>COUNTIF(H2:H51,"&gt;0")</f>
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="I55" s="8">
         <f>COUNTIF(I2:I51,"&gt;0")</f>
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="J55" s="8">
         <f>COUNTIF(J2:J51,"&gt;0")</f>
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="K55" s="7"/>
       <c r="L55" s="7"/>
@@ -30640,7 +30656,7 @@
 
 <file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:N56"/>
+  <dimension ref="A1:N57"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -30769,92 +30785,92 @@
       <c r="N3" s="56"/>
     </row>
     <row r="4" ht="15" customHeight="1">
-      <c r="A4" t="s" s="5">
+      <c r="A4" t="s" s="53">
+        <v>16</v>
+      </c>
+      <c r="B4" t="s" s="53">
+        <v>17</v>
+      </c>
+      <c r="C4" s="54">
+        <v>37731</v>
+      </c>
+      <c r="D4" s="54">
+        <v>8838</v>
+      </c>
+      <c r="E4" s="54">
+        <v>7897</v>
+      </c>
+      <c r="F4" s="54">
+        <v>5861</v>
+      </c>
+      <c r="G4" s="54">
+        <v>2036</v>
+      </c>
+      <c r="H4" s="54">
+        <v>941</v>
+      </c>
+      <c r="I4" s="54">
+        <v>499</v>
+      </c>
+      <c r="J4" s="54">
+        <v>442</v>
+      </c>
+      <c r="K4" s="56"/>
+      <c r="L4" s="56"/>
+      <c r="M4" s="56"/>
+      <c r="N4" s="56"/>
+    </row>
+    <row r="5" ht="15" customHeight="1">
+      <c r="A5" t="s" s="5">
         <v>14</v>
       </c>
-      <c r="B4" t="s" s="5">
+      <c r="B5" t="s" s="5">
         <v>15</v>
       </c>
-      <c r="C4" s="6">
+      <c r="C5" s="6">
         <v>15079</v>
       </c>
-      <c r="D4" s="6">
+      <c r="D5" s="6">
         <v>6942</v>
       </c>
-      <c r="E4" s="6">
+      <c r="E5" s="6">
         <v>2436</v>
       </c>
-      <c r="F4" s="6">
+      <c r="F5" s="6">
         <v>2019</v>
       </c>
-      <c r="G4" s="6">
+      <c r="G5" s="6">
         <v>417</v>
       </c>
-      <c r="H4" s="6">
+      <c r="H5" s="6">
         <v>4506</v>
       </c>
-      <c r="I4" s="6">
+      <c r="I5" s="6">
         <v>3472</v>
       </c>
-      <c r="J4" s="6">
+      <c r="J5" s="6">
         <v>1034</v>
       </c>
-      <c r="K4" s="7"/>
-      <c r="L4" s="7"/>
-      <c r="M4" s="7"/>
-      <c r="N4" s="7"/>
-    </row>
-    <row r="5" ht="15" customHeight="1" hidden="1">
-      <c r="A5" t="s" s="5">
-        <v>16</v>
-      </c>
-      <c r="B5" t="s" s="5">
-        <v>17</v>
-      </c>
-      <c r="C5" s="6"/>
-      <c r="D5" s="6"/>
-      <c r="E5" s="6"/>
-      <c r="F5" s="6"/>
-      <c r="G5" s="6"/>
-      <c r="H5" s="6"/>
-      <c r="I5" s="6"/>
-      <c r="J5" s="6"/>
       <c r="K5" s="7"/>
       <c r="L5" s="7"/>
       <c r="M5" s="7"/>
       <c r="N5" s="7"/>
     </row>
-    <row r="6" ht="15" customHeight="1">
+    <row r="6" ht="15" customHeight="1" hidden="1">
       <c r="A6" t="s" s="5">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B6" t="s" s="5">
-        <v>19</v>
-      </c>
-      <c r="C6" s="6">
-        <v>113229</v>
-      </c>
-      <c r="D6" s="6">
-        <v>27110</v>
-      </c>
-      <c r="E6" s="6">
-        <v>8258</v>
-      </c>
-      <c r="F6" s="6">
-        <v>6002</v>
-      </c>
-      <c r="G6" s="6">
-        <v>2256</v>
-      </c>
-      <c r="H6" s="6">
-        <v>18852</v>
-      </c>
-      <c r="I6" s="6">
-        <v>18768</v>
-      </c>
-      <c r="J6" s="6">
-        <v>84</v>
-      </c>
+        <v>17</v>
+      </c>
+      <c r="C6" s="6"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="6"/>
+      <c r="F6" s="6"/>
+      <c r="G6" s="6"/>
+      <c r="H6" s="6"/>
+      <c r="I6" s="6"/>
+      <c r="J6" s="6"/>
       <c r="K6" s="7"/>
       <c r="L6" s="7"/>
       <c r="M6" s="7"/>
@@ -30862,34 +30878,34 @@
     </row>
     <row r="7" ht="15" customHeight="1">
       <c r="A7" t="s" s="5">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B7" t="s" s="5">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C7" s="6">
-        <v>17441</v>
+        <v>113229</v>
       </c>
       <c r="D7" s="6">
-        <v>3270</v>
+        <v>27110</v>
       </c>
       <c r="E7" s="6">
-        <v>64</v>
+        <v>8258</v>
       </c>
       <c r="F7" s="6">
-        <v>45</v>
+        <v>6002</v>
       </c>
       <c r="G7" s="6">
-        <v>19</v>
+        <v>2256</v>
       </c>
       <c r="H7" s="6">
-        <v>3206</v>
+        <v>18852</v>
       </c>
       <c r="I7" s="6">
-        <v>2327</v>
+        <v>18768</v>
       </c>
       <c r="J7" s="6">
-        <v>879</v>
+        <v>84</v>
       </c>
       <c r="K7" s="7"/>
       <c r="L7" s="7"/>
@@ -30897,136 +30913,136 @@
       <c r="N7" s="7"/>
     </row>
     <row r="8" ht="15" customHeight="1">
-      <c r="A8" t="s" s="53">
+      <c r="A8" t="s" s="5">
+        <v>20</v>
+      </c>
+      <c r="B8" t="s" s="5">
+        <v>21</v>
+      </c>
+      <c r="C8" s="6">
+        <v>17441</v>
+      </c>
+      <c r="D8" s="6">
+        <v>3270</v>
+      </c>
+      <c r="E8" s="6">
+        <v>64</v>
+      </c>
+      <c r="F8" s="6">
+        <v>45</v>
+      </c>
+      <c r="G8" s="6">
+        <v>19</v>
+      </c>
+      <c r="H8" s="6">
+        <v>3206</v>
+      </c>
+      <c r="I8" s="6">
+        <v>2327</v>
+      </c>
+      <c r="J8" s="6">
+        <v>879</v>
+      </c>
+      <c r="K8" s="7"/>
+      <c r="L8" s="7"/>
+      <c r="M8" s="7"/>
+      <c r="N8" s="7"/>
+    </row>
+    <row r="9" ht="15" customHeight="1">
+      <c r="A9" t="s" s="53">
         <v>22</v>
       </c>
-      <c r="B8" t="s" s="53">
+      <c r="B9" t="s" s="53">
         <v>23</v>
       </c>
-      <c r="C8" s="54">
+      <c r="C9" s="54">
         <v>9111</v>
       </c>
-      <c r="D8" s="54"/>
-      <c r="E8" s="54"/>
-      <c r="F8" s="54"/>
-      <c r="G8" s="54"/>
-      <c r="H8" s="54"/>
-      <c r="I8" s="54"/>
-      <c r="J8" s="54"/>
-      <c r="K8" s="56"/>
-      <c r="L8" s="56"/>
-      <c r="M8" s="56"/>
-      <c r="N8" s="56"/>
-    </row>
-    <row r="9" ht="15" customHeight="1">
-      <c r="A9" t="s" s="5">
-        <v>24</v>
-      </c>
-      <c r="B9" t="s" s="5">
-        <v>25</v>
-      </c>
-      <c r="C9" s="6">
-        <v>3903</v>
-      </c>
-      <c r="D9" s="6"/>
-      <c r="E9" s="6"/>
-      <c r="F9" s="6"/>
-      <c r="G9" s="6"/>
-      <c r="H9" s="6"/>
-      <c r="I9" s="6"/>
-      <c r="J9" s="6"/>
-      <c r="K9" s="7"/>
-      <c r="L9" s="7"/>
-      <c r="M9" s="7"/>
-      <c r="N9" s="7"/>
+      <c r="D9" s="54"/>
+      <c r="E9" s="54"/>
+      <c r="F9" s="54"/>
+      <c r="G9" s="54"/>
+      <c r="H9" s="54"/>
+      <c r="I9" s="54"/>
+      <c r="J9" s="54"/>
+      <c r="K9" s="56"/>
+      <c r="L9" s="56"/>
+      <c r="M9" s="56"/>
+      <c r="N9" s="56"/>
     </row>
     <row r="10" ht="15" customHeight="1">
       <c r="A10" t="s" s="5">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B10" t="s" s="5">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C10" s="6">
-        <v>87736</v>
-      </c>
-      <c r="D10" s="6">
-        <v>13921</v>
-      </c>
-      <c r="E10" s="6">
-        <v>13247</v>
-      </c>
-      <c r="F10" s="6">
-        <v>8114</v>
-      </c>
-      <c r="G10" s="6">
-        <v>5133</v>
-      </c>
-      <c r="H10" s="6">
-        <v>674</v>
-      </c>
-      <c r="I10" s="6">
-        <v>320</v>
-      </c>
-      <c r="J10" s="6">
-        <v>354</v>
-      </c>
+        <v>3903</v>
+      </c>
+      <c r="D10" s="6"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="6"/>
+      <c r="G10" s="6"/>
+      <c r="H10" s="6"/>
+      <c r="I10" s="6"/>
+      <c r="J10" s="6"/>
       <c r="K10" s="7"/>
       <c r="L10" s="7"/>
       <c r="M10" s="7"/>
       <c r="N10" s="7"/>
     </row>
-    <row r="11" ht="15" customHeight="1" hidden="1">
+    <row r="11" ht="15" customHeight="1">
       <c r="A11" t="s" s="5">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B11" t="s" s="5">
-        <v>29</v>
-      </c>
-      <c r="C11" s="6"/>
-      <c r="D11" s="6"/>
-      <c r="E11" s="6"/>
-      <c r="F11" s="6"/>
-      <c r="G11" s="6"/>
-      <c r="H11" s="6"/>
-      <c r="I11" s="6"/>
-      <c r="J11" s="6"/>
+        <v>27</v>
+      </c>
+      <c r="C11" s="6">
+        <v>87736</v>
+      </c>
+      <c r="D11" s="6">
+        <v>13921</v>
+      </c>
+      <c r="E11" s="6">
+        <v>13247</v>
+      </c>
+      <c r="F11" s="6">
+        <v>8114</v>
+      </c>
+      <c r="G11" s="6">
+        <v>5133</v>
+      </c>
+      <c r="H11" s="6">
+        <v>674</v>
+      </c>
+      <c r="I11" s="6">
+        <v>320</v>
+      </c>
+      <c r="J11" s="6">
+        <v>354</v>
+      </c>
       <c r="K11" s="7"/>
       <c r="L11" s="7"/>
       <c r="M11" s="7"/>
       <c r="N11" s="7"/>
     </row>
-    <row r="12" ht="15" customHeight="1">
+    <row r="12" ht="15" customHeight="1" hidden="1">
       <c r="A12" t="s" s="5">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B12" t="s" s="5">
-        <v>31</v>
-      </c>
-      <c r="C12" s="6">
-        <v>3485</v>
-      </c>
-      <c r="D12" s="6">
-        <v>1120</v>
-      </c>
-      <c r="E12" s="6">
-        <v>370</v>
-      </c>
-      <c r="F12" s="6">
-        <v>276</v>
-      </c>
-      <c r="G12" s="6">
-        <v>94</v>
-      </c>
-      <c r="H12" s="6">
-        <v>750</v>
-      </c>
-      <c r="I12" s="6">
-        <v>612</v>
-      </c>
-      <c r="J12" s="6">
-        <v>138</v>
-      </c>
+        <v>29</v>
+      </c>
+      <c r="C12" s="6"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="6"/>
+      <c r="G12" s="6"/>
+      <c r="H12" s="6"/>
+      <c r="I12" s="6"/>
+      <c r="J12" s="6"/>
       <c r="K12" s="7"/>
       <c r="L12" s="7"/>
       <c r="M12" s="7"/>
@@ -31034,34 +31050,34 @@
     </row>
     <row r="13" ht="15" customHeight="1">
       <c r="A13" t="s" s="5">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B13" t="s" s="5">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C13" s="6">
-        <v>7528</v>
+        <v>3485</v>
       </c>
       <c r="D13" s="6">
-        <v>2387</v>
+        <v>1120</v>
       </c>
       <c r="E13" s="6">
-        <v>1468</v>
+        <v>370</v>
       </c>
       <c r="F13" s="6">
-        <v>797</v>
+        <v>276</v>
       </c>
       <c r="G13" s="6">
-        <v>671</v>
+        <v>94</v>
       </c>
       <c r="H13" s="6">
-        <v>919</v>
+        <v>750</v>
       </c>
       <c r="I13" s="6">
-        <v>635</v>
+        <v>612</v>
       </c>
       <c r="J13" s="6">
-        <v>284</v>
+        <v>138</v>
       </c>
       <c r="K13" s="7"/>
       <c r="L13" s="7"/>
@@ -31069,65 +31085,71 @@
       <c r="N13" s="7"/>
     </row>
     <row r="14" ht="15" customHeight="1">
-      <c r="A14" t="s" s="53">
-        <v>34</v>
-      </c>
-      <c r="B14" t="s" s="53">
-        <v>35</v>
-      </c>
-      <c r="C14" s="54">
-        <v>8025</v>
-      </c>
-      <c r="D14" s="54">
-        <v>3924</v>
-      </c>
-      <c r="E14" s="54">
-        <v>2730</v>
-      </c>
-      <c r="F14" s="54">
-        <v>2181</v>
-      </c>
-      <c r="G14" s="54">
-        <v>549</v>
-      </c>
-      <c r="H14" s="54">
-        <v>1194</v>
-      </c>
-      <c r="I14" s="54">
-        <v>1023</v>
-      </c>
-      <c r="J14" s="54">
-        <v>171</v>
-      </c>
-      <c r="K14" s="56"/>
-      <c r="L14" s="56"/>
-      <c r="M14" s="56"/>
-      <c r="N14" s="56"/>
+      <c r="A14" t="s" s="5">
+        <v>32</v>
+      </c>
+      <c r="B14" t="s" s="5">
+        <v>33</v>
+      </c>
+      <c r="C14" s="6">
+        <v>7528</v>
+      </c>
+      <c r="D14" s="6">
+        <v>2387</v>
+      </c>
+      <c r="E14" s="6">
+        <v>1468</v>
+      </c>
+      <c r="F14" s="6">
+        <v>797</v>
+      </c>
+      <c r="G14" s="6">
+        <v>671</v>
+      </c>
+      <c r="H14" s="6">
+        <v>919</v>
+      </c>
+      <c r="I14" s="6">
+        <v>635</v>
+      </c>
+      <c r="J14" s="6">
+        <v>284</v>
+      </c>
+      <c r="K14" s="7"/>
+      <c r="L14" s="7"/>
+      <c r="M14" s="7"/>
+      <c r="N14" s="7"/>
     </row>
     <row r="15" ht="15" customHeight="1">
       <c r="A15" t="s" s="53">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B15" t="s" s="53">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C15" s="54">
-        <v>29224</v>
+        <v>8025</v>
       </c>
       <c r="D15" s="54">
-        <v>4033</v>
-      </c>
-      <c r="E15" s="54"/>
-      <c r="F15" s="54"/>
-      <c r="G15" s="54"/>
+        <v>3924</v>
+      </c>
+      <c r="E15" s="54">
+        <v>2730</v>
+      </c>
+      <c r="F15" s="54">
+        <v>2181</v>
+      </c>
+      <c r="G15" s="54">
+        <v>549</v>
+      </c>
       <c r="H15" s="54">
-        <v>4033</v>
+        <v>1194</v>
       </c>
       <c r="I15" s="54">
-        <v>1536</v>
+        <v>1023</v>
       </c>
       <c r="J15" s="54">
-        <v>2497</v>
+        <v>171</v>
       </c>
       <c r="K15" s="56"/>
       <c r="L15" s="56"/>
@@ -31135,128 +31157,138 @@
       <c r="N15" s="56"/>
     </row>
     <row r="16" ht="15" customHeight="1">
-      <c r="A16" t="s" s="5">
+      <c r="A16" t="s" s="53">
+        <v>36</v>
+      </c>
+      <c r="B16" t="s" s="53">
+        <v>37</v>
+      </c>
+      <c r="C16" s="54">
+        <v>29224</v>
+      </c>
+      <c r="D16" s="54">
+        <v>4033</v>
+      </c>
+      <c r="E16" s="54"/>
+      <c r="F16" s="54"/>
+      <c r="G16" s="54"/>
+      <c r="H16" s="54">
+        <v>4033</v>
+      </c>
+      <c r="I16" s="54">
+        <v>1536</v>
+      </c>
+      <c r="J16" s="54">
+        <v>2497</v>
+      </c>
+      <c r="K16" s="56"/>
+      <c r="L16" s="56"/>
+      <c r="M16" s="56"/>
+      <c r="N16" s="56"/>
+    </row>
+    <row r="17" ht="15" customHeight="1">
+      <c r="A17" t="s" s="5">
         <v>38</v>
       </c>
-      <c r="B16" t="s" s="5">
+      <c r="B17" t="s" s="5">
         <v>39</v>
       </c>
-      <c r="C16" s="6">
+      <c r="C17" s="6">
         <v>25385</v>
       </c>
-      <c r="D16" s="6">
+      <c r="D17" s="6">
         <v>2821</v>
       </c>
-      <c r="E16" s="6">
+      <c r="E17" s="6">
         <v>736</v>
       </c>
-      <c r="F16" s="6">
+      <c r="F17" s="6">
         <v>689</v>
       </c>
-      <c r="G16" s="6">
+      <c r="G17" s="6">
         <v>47</v>
       </c>
-      <c r="H16" s="6">
+      <c r="H17" s="6">
         <v>2085</v>
       </c>
-      <c r="I16" s="6">
+      <c r="I17" s="6">
         <v>988</v>
       </c>
-      <c r="J16" s="6">
+      <c r="J17" s="6">
         <v>1097</v>
       </c>
-      <c r="K16" s="7"/>
-      <c r="L16" s="7"/>
-      <c r="M16" s="7"/>
-      <c r="N16" s="7"/>
-    </row>
-    <row r="17" ht="15" customHeight="1">
-      <c r="A17" t="s" s="53">
+      <c r="K17" s="7"/>
+      <c r="L17" s="7"/>
+      <c r="M17" s="7"/>
+      <c r="N17" s="7"/>
+    </row>
+    <row r="18" ht="15" customHeight="1">
+      <c r="A18" t="s" s="53">
         <v>40</v>
       </c>
-      <c r="B17" t="s" s="53">
+      <c r="B18" t="s" s="53">
         <v>41</v>
       </c>
-      <c r="C17" s="54">
+      <c r="C18" s="54">
         <v>8869</v>
       </c>
-      <c r="D17" s="54">
+      <c r="D18" s="54">
         <v>2590</v>
       </c>
-      <c r="E17" s="54">
+      <c r="E18" s="54">
         <v>1807</v>
       </c>
-      <c r="F17" s="54">
+      <c r="F18" s="54">
         <v>790</v>
       </c>
-      <c r="G17" s="54">
+      <c r="G18" s="54">
         <v>1001</v>
       </c>
-      <c r="H17" s="54">
+      <c r="H18" s="54">
         <v>783</v>
       </c>
-      <c r="I17" s="54">
+      <c r="I18" s="54">
         <v>548</v>
       </c>
-      <c r="J17" s="54">
+      <c r="J18" s="54">
         <v>235</v>
       </c>
-      <c r="K17" s="56"/>
-      <c r="L17" s="56"/>
-      <c r="M17" s="56"/>
-      <c r="N17" s="56"/>
-    </row>
-    <row r="18" ht="15" customHeight="1">
-      <c r="A18" t="s" s="5">
+      <c r="K18" s="56"/>
+      <c r="L18" s="56"/>
+      <c r="M18" s="56"/>
+      <c r="N18" s="56"/>
+    </row>
+    <row r="19" ht="15" customHeight="1">
+      <c r="A19" t="s" s="5">
         <v>44</v>
       </c>
-      <c r="B18" t="s" s="5">
+      <c r="B19" t="s" s="5">
         <v>45</v>
       </c>
-      <c r="C18" s="6">
+      <c r="C19" s="6">
         <v>27010</v>
       </c>
-      <c r="D18" s="6">
+      <c r="D19" s="6">
         <v>7754</v>
       </c>
-      <c r="E18" s="6">
+      <c r="E19" s="6">
         <v>2691</v>
       </c>
-      <c r="F18" s="6">
+      <c r="F19" s="6">
         <v>844</v>
       </c>
-      <c r="G18" s="6">
+      <c r="G19" s="6">
         <v>1847</v>
       </c>
-      <c r="H18" s="6">
+      <c r="H19" s="6">
         <v>5063</v>
       </c>
-      <c r="I18" s="6">
+      <c r="I19" s="6">
         <v>4284</v>
       </c>
-      <c r="J18" s="6">
+      <c r="J19" s="6">
         <v>779</v>
       </c>
-      <c r="K18" s="7"/>
-      <c r="L18" s="7"/>
-      <c r="M18" s="7"/>
-      <c r="N18" s="7"/>
-    </row>
-    <row r="19" ht="15" customHeight="1" hidden="1">
-      <c r="A19" t="s" s="5">
-        <v>42</v>
-      </c>
-      <c r="B19" t="s" s="5">
-        <v>43</v>
-      </c>
-      <c r="C19" s="6"/>
-      <c r="D19" s="6"/>
-      <c r="E19" s="6"/>
-      <c r="F19" s="6"/>
-      <c r="G19" s="6"/>
-      <c r="H19" s="6"/>
-      <c r="I19" s="6"/>
-      <c r="J19" s="6"/>
       <c r="K19" s="7"/>
       <c r="L19" s="7"/>
       <c r="M19" s="7"/>
@@ -31264,10 +31296,10 @@
     </row>
     <row r="20" ht="15" customHeight="1" hidden="1">
       <c r="A20" t="s" s="5">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B20" t="s" s="5">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C20" s="6"/>
       <c r="D20" s="6"/>
@@ -31282,33 +31314,21 @@
       <c r="M20" s="7"/>
       <c r="N20" s="7"/>
     </row>
-    <row r="21" ht="15" customHeight="1">
+    <row r="21" ht="15" customHeight="1" hidden="1">
       <c r="A21" t="s" s="5">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B21" t="s" s="5">
-        <v>47</v>
-      </c>
-      <c r="C21" s="6">
-        <v>6791</v>
-      </c>
-      <c r="D21" s="6">
-        <v>160</v>
-      </c>
-      <c r="E21" s="6">
-        <v>9</v>
-      </c>
+        <v>45</v>
+      </c>
+      <c r="C21" s="6"/>
+      <c r="D21" s="6"/>
+      <c r="E21" s="6"/>
       <c r="F21" s="6"/>
       <c r="G21" s="6"/>
-      <c r="H21" s="6">
-        <v>151</v>
-      </c>
-      <c r="I21" s="6">
-        <v>73</v>
-      </c>
-      <c r="J21" s="6">
-        <v>78</v>
-      </c>
+      <c r="H21" s="6"/>
+      <c r="I21" s="6"/>
+      <c r="J21" s="6"/>
       <c r="K21" s="7"/>
       <c r="L21" s="7"/>
       <c r="M21" s="7"/>
@@ -31316,110 +31336,108 @@
     </row>
     <row r="22" ht="15" customHeight="1">
       <c r="A22" t="s" s="5">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B22" t="s" s="5">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C22" s="6">
-        <v>18607</v>
+        <v>6791</v>
       </c>
       <c r="D22" s="6">
-        <v>1530</v>
+        <v>160</v>
       </c>
       <c r="E22" s="6">
-        <v>820</v>
+        <v>9</v>
       </c>
       <c r="F22" s="6"/>
       <c r="G22" s="6"/>
       <c r="H22" s="6">
-        <v>710</v>
-      </c>
-      <c r="I22" s="6"/>
-      <c r="J22" s="6"/>
+        <v>151</v>
+      </c>
+      <c r="I22" s="6">
+        <v>73</v>
+      </c>
+      <c r="J22" s="6">
+        <v>78</v>
+      </c>
       <c r="K22" s="7"/>
       <c r="L22" s="7"/>
       <c r="M22" s="7"/>
       <c r="N22" s="7"/>
     </row>
     <row r="23" ht="15" customHeight="1">
-      <c r="A23" t="s" s="53">
+      <c r="A23" t="s" s="5">
+        <v>48</v>
+      </c>
+      <c r="B23" t="s" s="5">
+        <v>49</v>
+      </c>
+      <c r="C23" s="6">
+        <v>18607</v>
+      </c>
+      <c r="D23" s="6">
+        <v>1530</v>
+      </c>
+      <c r="E23" s="6">
+        <v>820</v>
+      </c>
+      <c r="F23" s="6"/>
+      <c r="G23" s="6"/>
+      <c r="H23" s="6">
+        <v>710</v>
+      </c>
+      <c r="I23" s="6"/>
+      <c r="J23" s="6"/>
+      <c r="K23" s="7"/>
+      <c r="L23" s="7"/>
+      <c r="M23" s="7"/>
+      <c r="N23" s="7"/>
+    </row>
+    <row r="24" ht="15" customHeight="1">
+      <c r="A24" t="s" s="53">
         <v>50</v>
       </c>
-      <c r="B23" t="s" s="53">
+      <c r="B24" t="s" s="53">
         <v>51</v>
       </c>
-      <c r="C23" s="54">
+      <c r="C24" s="54">
         <v>1715</v>
       </c>
-      <c r="D23" s="54"/>
-      <c r="E23" s="54"/>
-      <c r="F23" s="54"/>
-      <c r="G23" s="54"/>
-      <c r="H23" s="54"/>
-      <c r="I23" s="54"/>
-      <c r="J23" s="54"/>
-      <c r="K23" s="56"/>
-      <c r="L23" s="56"/>
-      <c r="M23" s="56"/>
-      <c r="N23" s="56"/>
-    </row>
-    <row r="24" ht="15" customHeight="1">
-      <c r="A24" t="s" s="5">
-        <v>52</v>
-      </c>
-      <c r="B24" t="s" s="5">
-        <v>53</v>
-      </c>
-      <c r="C24" s="6">
-        <v>35425</v>
-      </c>
-      <c r="D24" s="6">
-        <v>1226</v>
-      </c>
-      <c r="E24" s="6"/>
-      <c r="F24" s="6"/>
-      <c r="G24" s="6"/>
-      <c r="H24" s="6">
-        <v>1226</v>
-      </c>
-      <c r="I24" s="6"/>
-      <c r="J24" s="6">
-        <v>1226</v>
-      </c>
-      <c r="K24" s="7"/>
-      <c r="L24" s="7"/>
-      <c r="M24" s="7"/>
-      <c r="N24" s="7"/>
+      <c r="D24" s="54"/>
+      <c r="E24" s="54"/>
+      <c r="F24" s="54"/>
+      <c r="G24" s="54"/>
+      <c r="H24" s="54"/>
+      <c r="I24" s="54"/>
+      <c r="J24" s="54"/>
+      <c r="K24" s="56"/>
+      <c r="L24" s="56"/>
+      <c r="M24" s="56"/>
+      <c r="N24" s="56"/>
     </row>
     <row r="25" ht="15" customHeight="1">
       <c r="A25" t="s" s="5">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B25" t="s" s="5">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C25" s="6">
-        <v>8330</v>
+        <v>35425</v>
       </c>
       <c r="D25" s="6">
-        <v>2166</v>
-      </c>
-      <c r="E25" s="6">
-        <v>973</v>
-      </c>
+        <v>1226</v>
+      </c>
+      <c r="E25" s="6"/>
       <c r="F25" s="6"/>
-      <c r="G25" s="6">
-        <v>973</v>
-      </c>
+      <c r="G25" s="6"/>
       <c r="H25" s="6">
-        <v>1193</v>
-      </c>
-      <c r="I25" s="6">
-        <v>533</v>
-      </c>
+        <v>1226</v>
+      </c>
+      <c r="I25" s="6"/>
       <c r="J25" s="6">
-        <v>660</v>
+        <v>1226</v>
       </c>
       <c r="K25" s="7"/>
       <c r="L25" s="7"/>
@@ -31427,232 +31445,246 @@
       <c r="N25" s="7"/>
     </row>
     <row r="26" ht="15" customHeight="1">
-      <c r="A26" t="s" s="53">
+      <c r="A26" t="s" s="5">
+        <v>54</v>
+      </c>
+      <c r="B26" t="s" s="5">
+        <v>55</v>
+      </c>
+      <c r="C26" s="6">
+        <v>8330</v>
+      </c>
+      <c r="D26" s="6">
+        <v>2166</v>
+      </c>
+      <c r="E26" s="6">
+        <v>973</v>
+      </c>
+      <c r="F26" s="6"/>
+      <c r="G26" s="6">
+        <v>973</v>
+      </c>
+      <c r="H26" s="6">
+        <v>1193</v>
+      </c>
+      <c r="I26" s="6">
+        <v>533</v>
+      </c>
+      <c r="J26" s="6">
+        <v>660</v>
+      </c>
+      <c r="K26" s="7"/>
+      <c r="L26" s="7"/>
+      <c r="M26" s="7"/>
+      <c r="N26" s="7"/>
+    </row>
+    <row r="27" ht="15" customHeight="1">
+      <c r="A27" t="s" s="53">
         <v>56</v>
       </c>
-      <c r="B26" t="s" s="53">
+      <c r="B27" t="s" s="53">
         <v>57</v>
       </c>
-      <c r="C26" s="54">
+      <c r="C27" s="54">
         <v>23062</v>
       </c>
-      <c r="D26" s="54">
+      <c r="D27" s="54">
         <v>11904</v>
       </c>
-      <c r="E26" s="54">
+      <c r="E27" s="54">
         <v>78469</v>
       </c>
-      <c r="F26" s="54">
+      <c r="F27" s="54">
         <v>4850</v>
       </c>
-      <c r="G26" s="54">
+      <c r="G27" s="54">
         <v>2619</v>
       </c>
-      <c r="H26" s="54">
+      <c r="H27" s="54">
         <v>4435</v>
       </c>
-      <c r="I26" s="54">
+      <c r="I27" s="54">
         <v>2097</v>
       </c>
-      <c r="J26" s="54">
+      <c r="J27" s="54">
         <v>2338</v>
       </c>
-      <c r="K26" s="56"/>
-      <c r="L26" s="56"/>
-      <c r="M26" s="56"/>
-      <c r="N26" s="56"/>
-    </row>
-    <row r="27" ht="15" customHeight="1" hidden="1">
-      <c r="A27" t="s" s="5">
+      <c r="K27" s="56"/>
+      <c r="L27" s="56"/>
+      <c r="M27" s="56"/>
+      <c r="N27" s="56"/>
+    </row>
+    <row r="28" ht="15" customHeight="1" hidden="1">
+      <c r="A28" t="s" s="5">
         <v>58</v>
       </c>
-      <c r="B27" t="s" s="5">
+      <c r="B28" t="s" s="5">
         <v>59</v>
       </c>
-      <c r="C27" s="6"/>
-      <c r="D27" s="6"/>
-      <c r="E27" s="6"/>
-      <c r="F27" s="6"/>
-      <c r="G27" s="6"/>
-      <c r="H27" s="6"/>
-      <c r="I27" s="6"/>
-      <c r="J27" s="6"/>
-      <c r="K27" s="7"/>
-      <c r="L27" s="7"/>
-      <c r="M27" s="7"/>
-      <c r="N27" s="7"/>
-    </row>
-    <row r="28" ht="15" customHeight="1">
-      <c r="A28" t="s" s="5">
-        <v>60</v>
-      </c>
-      <c r="B28" t="s" s="5">
-        <v>61</v>
-      </c>
-      <c r="C28" s="6">
-        <v>2538</v>
-      </c>
-      <c r="D28" s="6">
-        <v>329</v>
-      </c>
-      <c r="E28" s="6">
-        <v>213</v>
-      </c>
-      <c r="F28" s="6">
-        <v>59</v>
-      </c>
-      <c r="G28" s="6">
-        <v>154</v>
-      </c>
-      <c r="H28" s="6">
-        <v>116</v>
-      </c>
-      <c r="I28" s="6">
-        <v>17</v>
-      </c>
-      <c r="J28" s="6">
-        <v>99</v>
-      </c>
+      <c r="C28" s="6"/>
+      <c r="D28" s="6"/>
+      <c r="E28" s="6"/>
+      <c r="F28" s="6"/>
+      <c r="G28" s="6"/>
+      <c r="H28" s="6"/>
+      <c r="I28" s="6"/>
+      <c r="J28" s="6"/>
       <c r="K28" s="7"/>
       <c r="L28" s="7"/>
       <c r="M28" s="7"/>
       <c r="N28" s="7"/>
     </row>
     <row r="29" ht="15" customHeight="1">
-      <c r="A29" t="s" s="53">
-        <v>62</v>
-      </c>
-      <c r="B29" t="s" s="53">
-        <v>63</v>
-      </c>
-      <c r="C29" s="54">
-        <v>23969</v>
-      </c>
-      <c r="D29" s="54">
-        <v>6974</v>
-      </c>
-      <c r="E29" s="54">
-        <v>3971</v>
-      </c>
-      <c r="F29" s="54">
-        <v>3771</v>
-      </c>
-      <c r="G29" s="54">
-        <v>200</v>
-      </c>
-      <c r="H29" s="54">
-        <v>3003</v>
-      </c>
-      <c r="I29" s="54">
-        <v>3000</v>
-      </c>
-      <c r="J29" s="54">
-        <v>3</v>
-      </c>
-      <c r="K29" s="56"/>
-      <c r="L29" s="56"/>
-      <c r="M29" s="56"/>
-      <c r="N29" s="56"/>
+      <c r="A29" t="s" s="5">
+        <v>60</v>
+      </c>
+      <c r="B29" t="s" s="5">
+        <v>61</v>
+      </c>
+      <c r="C29" s="6">
+        <v>2538</v>
+      </c>
+      <c r="D29" s="6">
+        <v>329</v>
+      </c>
+      <c r="E29" s="6">
+        <v>213</v>
+      </c>
+      <c r="F29" s="6">
+        <v>59</v>
+      </c>
+      <c r="G29" s="6">
+        <v>154</v>
+      </c>
+      <c r="H29" s="6">
+        <v>116</v>
+      </c>
+      <c r="I29" s="6">
+        <v>17</v>
+      </c>
+      <c r="J29" s="6">
+        <v>99</v>
+      </c>
+      <c r="K29" s="7"/>
+      <c r="L29" s="7"/>
+      <c r="M29" s="7"/>
+      <c r="N29" s="7"/>
     </row>
     <row r="30" ht="15" customHeight="1">
       <c r="A30" t="s" s="53">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B30" t="s" s="53">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C30" s="54">
-        <v>1401</v>
+        <v>23969</v>
       </c>
       <c r="D30" s="54">
-        <v>397</v>
+        <v>6974</v>
       </c>
       <c r="E30" s="54">
-        <v>267</v>
-      </c>
-      <c r="F30" s="54"/>
-      <c r="G30" s="54"/>
+        <v>3971</v>
+      </c>
+      <c r="F30" s="54">
+        <v>3771</v>
+      </c>
+      <c r="G30" s="54">
+        <v>200</v>
+      </c>
       <c r="H30" s="54">
-        <v>130</v>
-      </c>
-      <c r="I30" s="54"/>
-      <c r="J30" s="54"/>
+        <v>3003</v>
+      </c>
+      <c r="I30" s="54">
+        <v>3000</v>
+      </c>
+      <c r="J30" s="54">
+        <v>3</v>
+      </c>
       <c r="K30" s="56"/>
       <c r="L30" s="56"/>
       <c r="M30" s="56"/>
       <c r="N30" s="56"/>
     </row>
     <row r="31" ht="15" customHeight="1">
-      <c r="A31" t="s" s="5">
-        <v>66</v>
-      </c>
-      <c r="B31" t="s" s="5">
-        <v>67</v>
-      </c>
-      <c r="C31" s="6">
-        <v>5388</v>
-      </c>
-      <c r="D31" s="6"/>
-      <c r="E31" s="6"/>
-      <c r="F31" s="6"/>
-      <c r="G31" s="6"/>
-      <c r="H31" s="6"/>
-      <c r="I31" s="6"/>
-      <c r="J31" s="6"/>
-      <c r="K31" s="7"/>
-      <c r="L31" s="7"/>
-      <c r="M31" s="7"/>
-      <c r="N31" s="7"/>
+      <c r="A31" t="s" s="53">
+        <v>64</v>
+      </c>
+      <c r="B31" t="s" s="53">
+        <v>65</v>
+      </c>
+      <c r="C31" s="54">
+        <v>1401</v>
+      </c>
+      <c r="D31" s="54">
+        <v>397</v>
+      </c>
+      <c r="E31" s="54">
+        <v>267</v>
+      </c>
+      <c r="F31" s="54"/>
+      <c r="G31" s="54"/>
+      <c r="H31" s="54">
+        <v>130</v>
+      </c>
+      <c r="I31" s="54"/>
+      <c r="J31" s="54"/>
+      <c r="K31" s="56"/>
+      <c r="L31" s="56"/>
+      <c r="M31" s="56"/>
+      <c r="N31" s="56"/>
     </row>
     <row r="32" ht="15" customHeight="1">
       <c r="A32" t="s" s="5">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B32" t="s" s="5">
-        <v>69</v>
-      </c>
-      <c r="C32" s="8">
-        <v>2359</v>
-      </c>
-      <c r="D32" s="6">
-        <v>31</v>
-      </c>
-      <c r="E32" s="6">
-        <f>G32</f>
-        <v>5</v>
-      </c>
+        <v>67</v>
+      </c>
+      <c r="C32" s="6">
+        <v>5388</v>
+      </c>
+      <c r="D32" s="6"/>
+      <c r="E32" s="6"/>
       <c r="F32" s="6"/>
-      <c r="G32" s="6">
-        <v>5</v>
-      </c>
-      <c r="H32" s="6">
-        <f>J32</f>
-        <v>26</v>
-      </c>
+      <c r="G32" s="6"/>
+      <c r="H32" s="6"/>
       <c r="I32" s="6"/>
-      <c r="J32" s="6">
-        <v>26</v>
-      </c>
+      <c r="J32" s="6"/>
       <c r="K32" s="7"/>
       <c r="L32" s="7"/>
       <c r="M32" s="7"/>
       <c r="N32" s="7"/>
     </row>
-    <row r="33" ht="15" customHeight="1" hidden="1">
+    <row r="33" ht="15" customHeight="1">
       <c r="A33" t="s" s="5">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B33" t="s" s="5">
-        <v>71</v>
-      </c>
-      <c r="C33" s="6"/>
-      <c r="D33" s="6"/>
-      <c r="E33" s="6"/>
+        <v>69</v>
+      </c>
+      <c r="C33" s="8">
+        <v>2359</v>
+      </c>
+      <c r="D33" s="6">
+        <v>31</v>
+      </c>
+      <c r="E33" s="6">
+        <f>G33</f>
+        <v>5</v>
+      </c>
       <c r="F33" s="6"/>
-      <c r="G33" s="6"/>
-      <c r="H33" s="6"/>
+      <c r="G33" s="6">
+        <v>5</v>
+      </c>
+      <c r="H33" s="6">
+        <f>J33</f>
+        <v>26</v>
+      </c>
       <c r="I33" s="6"/>
-      <c r="J33" s="6"/>
+      <c r="J33" s="6">
+        <v>26</v>
+      </c>
       <c r="K33" s="7"/>
       <c r="L33" s="7"/>
       <c r="M33" s="7"/>
@@ -31660,10 +31692,10 @@
     </row>
     <row r="34" ht="15" customHeight="1" hidden="1">
       <c r="A34" t="s" s="5">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B34" t="s" s="5">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C34" s="6"/>
       <c r="D34" s="6"/>
@@ -31678,37 +31710,21 @@
       <c r="M34" s="7"/>
       <c r="N34" s="7"/>
     </row>
-    <row r="35" ht="15" customHeight="1">
+    <row r="35" ht="15" customHeight="1" hidden="1">
       <c r="A35" t="s" s="5">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B35" t="s" s="5">
-        <v>75</v>
-      </c>
-      <c r="C35" s="6">
-        <v>12254</v>
-      </c>
-      <c r="D35" s="6">
-        <v>2503</v>
-      </c>
-      <c r="E35" s="6">
-        <v>1698</v>
-      </c>
-      <c r="F35" s="6">
-        <v>209</v>
-      </c>
-      <c r="G35" s="6">
-        <v>1489</v>
-      </c>
-      <c r="H35" s="6">
-        <v>805</v>
-      </c>
-      <c r="I35" s="6">
-        <v>89</v>
-      </c>
-      <c r="J35" s="6">
-        <v>716</v>
-      </c>
+        <v>73</v>
+      </c>
+      <c r="C35" s="6"/>
+      <c r="D35" s="6"/>
+      <c r="E35" s="6"/>
+      <c r="F35" s="6"/>
+      <c r="G35" s="6"/>
+      <c r="H35" s="6"/>
+      <c r="I35" s="6"/>
+      <c r="J35" s="6"/>
       <c r="K35" s="7"/>
       <c r="L35" s="7"/>
       <c r="M35" s="7"/>
@@ -31716,76 +31732,82 @@
     </row>
     <row r="36" ht="15" customHeight="1">
       <c r="A36" t="s" s="5">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B36" t="s" s="5">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C36" s="6">
-        <v>38380</v>
+        <v>12254</v>
       </c>
       <c r="D36" s="6">
-        <v>7341</v>
-      </c>
-      <c r="E36" s="6"/>
-      <c r="F36" s="6"/>
-      <c r="G36" s="6"/>
+        <v>2503</v>
+      </c>
+      <c r="E36" s="6">
+        <v>1698</v>
+      </c>
+      <c r="F36" s="6">
+        <v>209</v>
+      </c>
+      <c r="G36" s="6">
+        <v>1489</v>
+      </c>
       <c r="H36" s="6">
-        <v>7341</v>
+        <v>805</v>
       </c>
       <c r="I36" s="6">
-        <v>5139</v>
+        <v>89</v>
       </c>
       <c r="J36" s="6">
-        <v>2202</v>
+        <v>716</v>
       </c>
       <c r="K36" s="7"/>
       <c r="L36" s="7"/>
       <c r="M36" s="7"/>
       <c r="N36" s="7"/>
     </row>
-    <row r="37" ht="15" customHeight="1" hidden="1">
+    <row r="37" ht="15" customHeight="1">
       <c r="A37" t="s" s="5">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B37" t="s" s="5">
-        <v>79</v>
-      </c>
-      <c r="C37" s="6"/>
-      <c r="D37" s="6"/>
+        <v>77</v>
+      </c>
+      <c r="C37" s="6">
+        <v>38380</v>
+      </c>
+      <c r="D37" s="6">
+        <v>7341</v>
+      </c>
       <c r="E37" s="6"/>
       <c r="F37" s="6"/>
       <c r="G37" s="6"/>
-      <c r="H37" s="6"/>
-      <c r="I37" s="6"/>
-      <c r="J37" s="6"/>
+      <c r="H37" s="6">
+        <v>7341</v>
+      </c>
+      <c r="I37" s="6">
+        <v>5139</v>
+      </c>
+      <c r="J37" s="6">
+        <v>2202</v>
+      </c>
       <c r="K37" s="7"/>
       <c r="L37" s="7"/>
       <c r="M37" s="7"/>
       <c r="N37" s="7"/>
     </row>
-    <row r="38" ht="15" customHeight="1">
+    <row r="38" ht="15" customHeight="1" hidden="1">
       <c r="A38" t="s" s="5">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B38" t="s" s="5">
-        <v>81</v>
-      </c>
-      <c r="C38" s="6">
-        <v>22628</v>
-      </c>
-      <c r="D38" s="6">
-        <v>1993</v>
-      </c>
-      <c r="E38" s="6">
-        <v>1993</v>
-      </c>
-      <c r="F38" s="6">
-        <v>763</v>
-      </c>
-      <c r="G38" s="6">
-        <v>1230</v>
-      </c>
+        <v>79</v>
+      </c>
+      <c r="C38" s="6"/>
+      <c r="D38" s="6"/>
+      <c r="E38" s="6"/>
+      <c r="F38" s="6"/>
+      <c r="G38" s="6"/>
       <c r="H38" s="6"/>
       <c r="I38" s="6"/>
       <c r="J38" s="6"/>
@@ -31796,35 +31818,29 @@
     </row>
     <row r="39" ht="15" customHeight="1">
       <c r="A39" t="s" s="5">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B39" t="s" s="5">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C39" s="6">
-        <v>14292</v>
+        <v>22628</v>
       </c>
       <c r="D39" s="6">
-        <v>1547</v>
+        <v>1993</v>
       </c>
       <c r="E39" s="6">
-        <v>1515</v>
+        <v>1993</v>
       </c>
       <c r="F39" s="6">
-        <v>770</v>
+        <v>763</v>
       </c>
       <c r="G39" s="6">
-        <v>745</v>
-      </c>
-      <c r="H39" s="6">
-        <v>32</v>
-      </c>
-      <c r="I39" s="6">
-        <v>6</v>
-      </c>
-      <c r="J39" s="6">
-        <v>26</v>
-      </c>
+        <v>1230</v>
+      </c>
+      <c r="H39" s="6"/>
+      <c r="I39" s="6"/>
+      <c r="J39" s="6"/>
       <c r="K39" s="7"/>
       <c r="L39" s="7"/>
       <c r="M39" s="7"/>
@@ -31832,113 +31848,129 @@
     </row>
     <row r="40" ht="15" customHeight="1">
       <c r="A40" t="s" s="5">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B40" t="s" s="5">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C40" s="6">
-        <v>42101</v>
+        <v>14292</v>
       </c>
       <c r="D40" s="6">
-        <v>5941</v>
-      </c>
-      <c r="E40" s="6"/>
-      <c r="F40" s="6"/>
-      <c r="G40" s="6"/>
+        <v>1547</v>
+      </c>
+      <c r="E40" s="6">
+        <v>1515</v>
+      </c>
+      <c r="F40" s="6">
+        <v>770</v>
+      </c>
+      <c r="G40" s="6">
+        <v>745</v>
+      </c>
       <c r="H40" s="6">
-        <v>5941</v>
+        <v>32</v>
       </c>
       <c r="I40" s="6">
-        <v>3656</v>
+        <v>6</v>
       </c>
       <c r="J40" s="6">
-        <v>2285</v>
+        <v>26</v>
       </c>
       <c r="K40" s="7"/>
       <c r="L40" s="7"/>
       <c r="M40" s="7"/>
       <c r="N40" s="7"/>
     </row>
-    <row r="41" ht="16.6" customHeight="1">
-      <c r="A41" t="s" s="53">
+    <row r="41" ht="15" customHeight="1">
+      <c r="A41" t="s" s="5">
+        <v>84</v>
+      </c>
+      <c r="B41" t="s" s="5">
+        <v>85</v>
+      </c>
+      <c r="C41" s="6">
+        <v>42101</v>
+      </c>
+      <c r="D41" s="6">
+        <v>5941</v>
+      </c>
+      <c r="E41" s="6"/>
+      <c r="F41" s="6"/>
+      <c r="G41" s="6"/>
+      <c r="H41" s="6">
+        <v>5941</v>
+      </c>
+      <c r="I41" s="6">
+        <v>3656</v>
+      </c>
+      <c r="J41" s="6">
+        <v>2285</v>
+      </c>
+      <c r="K41" s="7"/>
+      <c r="L41" s="7"/>
+      <c r="M41" s="7"/>
+      <c r="N41" s="7"/>
+    </row>
+    <row r="42" ht="16.6" customHeight="1">
+      <c r="A42" t="s" s="53">
         <v>86</v>
       </c>
-      <c r="B41" t="s" s="53">
+      <c r="B42" t="s" s="53">
         <v>87</v>
       </c>
-      <c r="C41" s="54">
+      <c r="C42" s="54">
         <v>1491</v>
       </c>
-      <c r="D41" s="54">
+      <c r="D42" s="54">
         <v>350</v>
       </c>
-      <c r="E41" s="54">
+      <c r="E42" s="54">
         <v>277</v>
       </c>
-      <c r="F41" s="54">
+      <c r="F42" s="54">
         <v>237</v>
       </c>
-      <c r="G41" s="54">
+      <c r="G42" s="54">
         <v>37</v>
       </c>
-      <c r="H41" s="54">
+      <c r="H42" s="54">
         <v>73</v>
       </c>
-      <c r="I41" s="54">
+      <c r="I42" s="54">
         <v>33</v>
       </c>
-      <c r="J41" s="54">
+      <c r="J42" s="54">
         <v>18</v>
       </c>
-      <c r="K41" t="s" s="87">
+      <c r="K42" t="s" s="87">
         <v>154</v>
       </c>
-      <c r="L41" s="56"/>
-      <c r="M41" s="56"/>
-      <c r="N41" s="56"/>
-    </row>
-    <row r="42" ht="15" customHeight="1">
-      <c r="A42" t="s" s="5">
+      <c r="L42" s="56"/>
+      <c r="M42" s="56"/>
+      <c r="N42" s="56"/>
+    </row>
+    <row r="43" ht="15" customHeight="1">
+      <c r="A43" t="s" s="5">
         <v>88</v>
       </c>
-      <c r="B42" t="s" s="5">
+      <c r="B43" t="s" s="5">
         <v>89</v>
       </c>
-      <c r="C42" s="6">
+      <c r="C43" s="6">
         <v>17318</v>
       </c>
-      <c r="D42" s="6">
+      <c r="D43" s="6">
         <v>2655</v>
       </c>
-      <c r="E42" s="6">
+      <c r="E43" s="6">
         <v>1480</v>
       </c>
-      <c r="F42" s="6"/>
-      <c r="G42" s="6"/>
-      <c r="H42" s="6">
-        <v>1175</v>
-      </c>
-      <c r="I42" s="6"/>
-      <c r="J42" s="6"/>
-      <c r="K42" s="7"/>
-      <c r="L42" s="7"/>
-      <c r="M42" s="7"/>
-      <c r="N42" s="7"/>
-    </row>
-    <row r="43" ht="15" customHeight="1" hidden="1">
-      <c r="A43" t="s" s="5">
-        <v>90</v>
-      </c>
-      <c r="B43" t="s" s="5">
-        <v>91</v>
-      </c>
-      <c r="C43" s="6"/>
-      <c r="D43" s="6"/>
-      <c r="E43" s="6"/>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
-      <c r="H43" s="6"/>
+      <c r="H43" s="6">
+        <v>1175</v>
+      </c>
       <c r="I43" s="6"/>
       <c r="J43" s="6"/>
       <c r="K43" s="7"/>
@@ -31946,16 +31978,14 @@
       <c r="M43" s="7"/>
       <c r="N43" s="7"/>
     </row>
-    <row r="44" ht="15" customHeight="1">
+    <row r="44" ht="15" customHeight="1" hidden="1">
       <c r="A44" t="s" s="5">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B44" t="s" s="5">
-        <v>93</v>
-      </c>
-      <c r="C44" s="6">
-        <v>21382</v>
-      </c>
+        <v>91</v>
+      </c>
+      <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
@@ -31968,14 +31998,16 @@
       <c r="M44" s="7"/>
       <c r="N44" s="7"/>
     </row>
-    <row r="45" ht="15" customHeight="1" hidden="1">
+    <row r="45" ht="15" customHeight="1">
       <c r="A45" t="s" s="5">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B45" t="s" s="5">
-        <v>95</v>
-      </c>
-      <c r="C45" s="6"/>
+        <v>93</v>
+      </c>
+      <c r="C45" s="6">
+        <v>21382</v>
+      </c>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
@@ -31988,27 +32020,19 @@
       <c r="M45" s="7"/>
       <c r="N45" s="7"/>
     </row>
-    <row r="46" ht="15" customHeight="1">
+    <row r="46" ht="15" customHeight="1" hidden="1">
       <c r="A46" t="s" s="5">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B46" t="s" s="5">
-        <v>97</v>
-      </c>
-      <c r="C46" s="6">
-        <v>5579</v>
-      </c>
-      <c r="D46" s="6">
-        <v>2652</v>
-      </c>
-      <c r="E46" s="6">
-        <v>1152</v>
-      </c>
+        <v>95</v>
+      </c>
+      <c r="C46" s="6"/>
+      <c r="D46" s="6"/>
+      <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="6">
-        <v>1500</v>
-      </c>
+      <c r="H46" s="6"/>
       <c r="I46" s="6"/>
       <c r="J46" s="6"/>
       <c r="K46" s="7"/>
@@ -32016,19 +32040,27 @@
       <c r="M46" s="7"/>
       <c r="N46" s="7"/>
     </row>
-    <row r="47" ht="15" customHeight="1" hidden="1">
+    <row r="47" ht="15" customHeight="1">
       <c r="A47" t="s" s="5">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B47" t="s" s="5">
-        <v>99</v>
-      </c>
-      <c r="C47" s="6"/>
-      <c r="D47" s="6"/>
-      <c r="E47" s="6"/>
+        <v>97</v>
+      </c>
+      <c r="C47" s="6">
+        <v>5579</v>
+      </c>
+      <c r="D47" s="6">
+        <v>2652</v>
+      </c>
+      <c r="E47" s="6">
+        <v>1152</v>
+      </c>
       <c r="F47" s="6"/>
       <c r="G47" s="6"/>
-      <c r="H47" s="6"/>
+      <c r="H47" s="6">
+        <v>1500</v>
+      </c>
       <c r="I47" s="6"/>
       <c r="J47" s="6"/>
       <c r="K47" s="7"/>
@@ -32036,29 +32068,19 @@
       <c r="M47" s="7"/>
       <c r="N47" s="7"/>
     </row>
-    <row r="48" ht="15" customHeight="1">
+    <row r="48" ht="15" customHeight="1" hidden="1">
       <c r="A48" t="s" s="5">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B48" t="s" s="5">
-        <v>101</v>
-      </c>
-      <c r="C48" s="8">
-        <v>1066</v>
-      </c>
-      <c r="D48" s="6">
-        <f>E48+H48</f>
-        <v>250</v>
-      </c>
-      <c r="E48" s="6">
-        <v>92</v>
-      </c>
+        <v>99</v>
+      </c>
+      <c r="C48" s="6"/>
+      <c r="D48" s="6"/>
+      <c r="E48" s="6"/>
       <c r="F48" s="6"/>
-      <c r="G48" s="7"/>
-      <c r="H48" s="6">
-        <f>27+131</f>
-        <v>158</v>
-      </c>
+      <c r="G48" s="6"/>
+      <c r="H48" s="6"/>
       <c r="I48" s="6"/>
       <c r="J48" s="6"/>
       <c r="K48" s="7"/>
@@ -32068,95 +32090,95 @@
     </row>
     <row r="49" ht="15" customHeight="1">
       <c r="A49" t="s" s="5">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B49" t="s" s="5">
-        <v>103</v>
-      </c>
-      <c r="C49" s="6">
-        <v>17330</v>
+        <v>101</v>
+      </c>
+      <c r="C49" s="8">
+        <v>1066</v>
       </c>
       <c r="D49" s="6">
-        <v>6054</v>
-      </c>
-      <c r="E49" s="6"/>
+        <f>E49+H49</f>
+        <v>250</v>
+      </c>
+      <c r="E49" s="6">
+        <v>92</v>
+      </c>
       <c r="F49" s="6"/>
-      <c r="G49" s="6"/>
+      <c r="G49" s="7"/>
       <c r="H49" s="6">
-        <v>6054</v>
-      </c>
-      <c r="I49" s="6">
-        <v>4064</v>
-      </c>
-      <c r="J49" s="6">
-        <v>1990</v>
-      </c>
+        <f>27+131</f>
+        <v>158</v>
+      </c>
+      <c r="I49" s="6"/>
+      <c r="J49" s="6"/>
       <c r="K49" s="7"/>
       <c r="L49" s="7"/>
       <c r="M49" s="7"/>
-      <c r="N49" s="6"/>
+      <c r="N49" s="7"/>
     </row>
     <row r="50" ht="15" customHeight="1">
       <c r="A50" t="s" s="5">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B50" t="s" s="5">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C50" s="6">
-        <v>23765</v>
+        <v>17330</v>
       </c>
       <c r="D50" s="6">
-        <v>12152</v>
-      </c>
-      <c r="E50" s="6">
-        <v>4676</v>
-      </c>
-      <c r="F50" s="6">
-        <v>2672</v>
-      </c>
-      <c r="G50" s="6">
-        <v>2004</v>
-      </c>
+        <v>6054</v>
+      </c>
+      <c r="E50" s="6"/>
+      <c r="F50" s="6"/>
+      <c r="G50" s="6"/>
       <c r="H50" s="6">
-        <v>7476</v>
+        <v>6054</v>
       </c>
       <c r="I50" s="6">
-        <v>3768</v>
+        <v>4064</v>
       </c>
       <c r="J50" s="6">
-        <v>3708</v>
+        <v>1990</v>
       </c>
       <c r="K50" s="7"/>
       <c r="L50" s="7"/>
       <c r="M50" s="7"/>
-      <c r="N50" s="7"/>
+      <c r="N50" s="6"/>
     </row>
     <row r="51" ht="15" customHeight="1">
       <c r="A51" t="s" s="5">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B51" t="s" s="5">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C51" s="6">
-        <v>6640</v>
+        <v>23765</v>
       </c>
       <c r="D51" s="6">
-        <v>865</v>
+        <v>12152</v>
       </c>
       <c r="E51" s="6">
-        <v>865</v>
+        <v>4676</v>
       </c>
       <c r="F51" s="6">
-        <v>65</v>
+        <v>2672</v>
       </c>
       <c r="G51" s="6">
-        <v>800</v>
-      </c>
-      <c r="H51" s="6"/>
-      <c r="I51" s="6"/>
-      <c r="J51" s="6"/>
+        <v>2004</v>
+      </c>
+      <c r="H51" s="6">
+        <v>7476</v>
+      </c>
+      <c r="I51" s="6">
+        <v>3768</v>
+      </c>
+      <c r="J51" s="6">
+        <v>3708</v>
+      </c>
       <c r="K51" s="7"/>
       <c r="L51" s="7"/>
       <c r="M51" s="7"/>
@@ -32164,51 +32186,65 @@
     </row>
     <row r="52" ht="15" customHeight="1">
       <c r="A52" t="s" s="5">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B52" t="s" s="5">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C52" s="6">
-        <v>2364</v>
+        <v>6640</v>
       </c>
       <c r="D52" s="6">
-        <v>681</v>
+        <v>865</v>
       </c>
       <c r="E52" s="6">
-        <v>482</v>
+        <v>865</v>
       </c>
       <c r="F52" s="6">
-        <v>24</v>
+        <v>65</v>
       </c>
       <c r="G52" s="6">
-        <v>458</v>
-      </c>
-      <c r="H52" s="6">
-        <v>199</v>
-      </c>
-      <c r="I52" s="6">
-        <v>72</v>
-      </c>
-      <c r="J52" s="6">
-        <v>127</v>
-      </c>
+        <v>800</v>
+      </c>
+      <c r="H52" s="6"/>
+      <c r="I52" s="6"/>
+      <c r="J52" s="6"/>
       <c r="K52" s="7"/>
       <c r="L52" s="7"/>
       <c r="M52" s="7"/>
       <c r="N52" s="7"/>
     </row>
     <row r="53" ht="15" customHeight="1">
-      <c r="A53" s="7"/>
-      <c r="B53" s="7"/>
-      <c r="C53" s="7"/>
-      <c r="D53" s="7"/>
-      <c r="E53" s="7"/>
-      <c r="F53" s="7"/>
-      <c r="G53" s="7"/>
-      <c r="H53" s="7"/>
-      <c r="I53" s="7"/>
-      <c r="J53" s="7"/>
+      <c r="A53" t="s" s="5">
+        <v>108</v>
+      </c>
+      <c r="B53" t="s" s="5">
+        <v>109</v>
+      </c>
+      <c r="C53" s="6">
+        <v>2364</v>
+      </c>
+      <c r="D53" s="6">
+        <v>681</v>
+      </c>
+      <c r="E53" s="6">
+        <v>482</v>
+      </c>
+      <c r="F53" s="6">
+        <v>24</v>
+      </c>
+      <c r="G53" s="6">
+        <v>458</v>
+      </c>
+      <c r="H53" s="6">
+        <v>199</v>
+      </c>
+      <c r="I53" s="6">
+        <v>72</v>
+      </c>
+      <c r="J53" s="6">
+        <v>127</v>
+      </c>
       <c r="K53" s="7"/>
       <c r="L53" s="7"/>
       <c r="M53" s="7"/>
@@ -32216,103 +32252,119 @@
     </row>
     <row r="54" ht="15" customHeight="1">
       <c r="A54" s="7"/>
-      <c r="B54" t="s" s="9">
-        <v>110</v>
-      </c>
-      <c r="C54" s="10">
-        <f>SUM(C2:C52)</f>
-        <v>742162</v>
-      </c>
-      <c r="D54" s="10">
-        <f>SUM(D2:D52)</f>
-        <v>147107</v>
-      </c>
-      <c r="E54" s="10">
-        <f>SUM(E2:E52)</f>
-        <v>134045</v>
-      </c>
-      <c r="F54" s="10">
-        <f>SUM(F2:F52)+E21+E22+E30+E42+E46+E48</f>
-        <v>39804</v>
-      </c>
-      <c r="G54" s="10">
-        <f>SUM(G2:G52)</f>
-        <v>23222</v>
-      </c>
-      <c r="H54" s="10">
-        <f>SUM(H2:H52)</f>
-        <v>84066</v>
-      </c>
-      <c r="I54" s="10">
-        <f>SUM(I2:I52)+H22+H30+H42+H46+H48</f>
-        <v>60892</v>
-      </c>
-      <c r="J54" s="10">
-        <f>SUM(J2:J52)</f>
-        <v>23153</v>
-      </c>
+      <c r="B54" s="7"/>
+      <c r="C54" s="7"/>
+      <c r="D54" s="7"/>
+      <c r="E54" s="7"/>
+      <c r="F54" s="7"/>
+      <c r="G54" s="7"/>
+      <c r="H54" s="7"/>
+      <c r="I54" s="7"/>
+      <c r="J54" s="7"/>
       <c r="K54" s="7"/>
-      <c r="L54" s="6"/>
+      <c r="L54" s="7"/>
       <c r="M54" s="7"/>
       <c r="N54" s="7"/>
     </row>
     <row r="55" ht="15" customHeight="1">
       <c r="A55" s="7"/>
-      <c r="B55" s="7"/>
-      <c r="C55" s="7"/>
-      <c r="D55" s="7"/>
-      <c r="E55" s="7"/>
-      <c r="F55" s="7"/>
-      <c r="G55" s="7"/>
-      <c r="H55" s="7"/>
-      <c r="I55" s="7"/>
-      <c r="J55" s="7"/>
+      <c r="B55" t="s" s="9">
+        <v>110</v>
+      </c>
+      <c r="C55" s="10">
+        <f>SUM(C2:C53)</f>
+        <v>779893</v>
+      </c>
+      <c r="D55" s="10">
+        <f>SUM(D2:D53)</f>
+        <v>155945</v>
+      </c>
+      <c r="E55" s="10">
+        <f>SUM(E2:E53)</f>
+        <v>141942</v>
+      </c>
+      <c r="F55" s="10">
+        <f>SUM(F2:F53)+E22+E23+E31+E43+E47+E49</f>
+        <v>45665</v>
+      </c>
+      <c r="G55" s="10">
+        <f>SUM(G2:G53)</f>
+        <v>25258</v>
+      </c>
+      <c r="H55" s="10">
+        <f>SUM(H2:H53)</f>
+        <v>85007</v>
+      </c>
+      <c r="I55" s="10">
+        <f>SUM(I2:I53)+H23+H31+H43+H47+H49</f>
+        <v>61391</v>
+      </c>
+      <c r="J55" s="10">
+        <f>SUM(J2:J53)</f>
+        <v>23595</v>
+      </c>
       <c r="K55" s="7"/>
-      <c r="L55" s="7"/>
+      <c r="L55" s="6"/>
       <c r="M55" s="7"/>
       <c r="N55" s="7"/>
     </row>
     <row r="56" ht="15" customHeight="1">
       <c r="A56" s="7"/>
-      <c r="B56" t="s" s="5">
-        <v>140</v>
-      </c>
-      <c r="C56" s="8">
-        <f>COUNTIF(C2:C52,"&gt;0")</f>
-        <v>40</v>
-      </c>
-      <c r="D56" s="8">
-        <f>COUNTIF(D2:D52,"&gt;0")</f>
-        <v>35</v>
-      </c>
-      <c r="E56" s="8">
-        <f>COUNTIF(E2:E52,"&gt;0")</f>
-        <v>30</v>
-      </c>
-      <c r="F56" s="8">
-        <f>COUNTIF(F2:F52,"&gt;0")</f>
-        <v>21</v>
-      </c>
-      <c r="G56" s="8">
-        <f>COUNTIF(G2:G52,"&gt;0")</f>
-        <v>24</v>
-      </c>
-      <c r="H56" s="8">
-        <f>COUNTIF(H2:H52,"&gt;0")</f>
-        <v>33</v>
-      </c>
-      <c r="I56" s="8">
-        <f>COUNTIF(I2:I52,"&gt;0")</f>
-        <v>25</v>
-      </c>
-      <c r="J56" s="8">
-        <f>COUNTIF(J2:J52,"&gt;0")</f>
-        <v>28</v>
-      </c>
+      <c r="B56" s="7"/>
+      <c r="C56" s="7"/>
+      <c r="D56" s="7"/>
+      <c r="E56" s="7"/>
+      <c r="F56" s="7"/>
+      <c r="G56" s="7"/>
+      <c r="H56" s="7"/>
+      <c r="I56" s="7"/>
+      <c r="J56" s="7"/>
       <c r="K56" s="7"/>
       <c r="L56" s="7"/>
       <c r="M56" s="7"/>
       <c r="N56" s="7"/>
+    </row>
+    <row r="57" ht="15" customHeight="1">
+      <c r="A57" s="7"/>
+      <c r="B57" t="s" s="5">
+        <v>140</v>
+      </c>
+      <c r="C57" s="8">
+        <f>COUNTIF(C2:C53,"&gt;0")</f>
+        <v>41</v>
+      </c>
+      <c r="D57" s="8">
+        <f>COUNTIF(D2:D53,"&gt;0")</f>
+        <v>36</v>
+      </c>
+      <c r="E57" s="8">
+        <f>COUNTIF(E2:E53,"&gt;0")</f>
+        <v>31</v>
+      </c>
+      <c r="F57" s="8">
+        <f>COUNTIF(F2:F53,"&gt;0")</f>
+        <v>22</v>
+      </c>
+      <c r="G57" s="8">
+        <f>COUNTIF(G2:G53,"&gt;0")</f>
+        <v>25</v>
+      </c>
+      <c r="H57" s="8">
+        <f>COUNTIF(H2:H53,"&gt;0")</f>
+        <v>34</v>
+      </c>
+      <c r="I57" s="8">
+        <f>COUNTIF(I2:I53,"&gt;0")</f>
+        <v>26</v>
+      </c>
+      <c r="J57" s="8">
+        <f>COUNTIF(J2:J53,"&gt;0")</f>
+        <v>29</v>
+      </c>
+      <c r="K57" s="7"/>
+      <c r="L57" s="7"/>
+      <c r="M57" s="7"/>
+      <c r="N57" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
add updated 2020 data to tables
</commit_message>
<xml_diff>
--- a/data/Data for web team 2020 v6 CORRECTED.xlsx
+++ b/data/Data for web team 2020 v6 CORRECTED.xlsx
@@ -31,12 +31,13 @@
     <sheet name="PopPercentages 2020" sheetId="24" r:id="rId27"/>
     <sheet name="State Notes 2020" sheetId="25" r:id="rId28"/>
     <sheet name="Survey 2020" sheetId="26" r:id="rId29"/>
+    <sheet name="Survey Submissions" sheetId="27" r:id="rId30"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="222">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="224">
   <si>
     <t>State Abbrev</t>
   </si>
@@ -787,6 +788,12 @@
   <si>
     <t>ALOS data include only the months from the most recent prison intake to prison exit. Months accumulated on multiple stays in prison on the same conviction (e.g., new intake, then parole release, then return from parole, then re-parole) are not included in the ALOS data contained here.</t>
   </si>
+  <si>
+    <t>Completed</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
 </sst>
 </file>
 
@@ -800,7 +807,7 @@
     <numFmt numFmtId="62" formatCode="&quot;$&quot;0.00"/>
     <numFmt numFmtId="63" formatCode="#,##0.0"/>
   </numFmts>
-  <fonts count="12">
+  <fonts count="15">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -860,7 +867,23 @@
       <name val="Calibri"/>
     </font>
     <font>
+      <sz val="14"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
       <sz val="12"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b val="1"/>
+      <sz val="14"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="14"/>
       <color indexed="8"/>
       <name val="Calibri"/>
     </font>
@@ -874,7 +897,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor indexed="10"/>
+        <fgColor indexed="9"/>
         <bgColor auto="1"/>
       </patternFill>
     </fill>
@@ -910,7 +933,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor indexed="17"/>
+        <fgColor indexed="18"/>
         <bgColor auto="1"/>
       </patternFill>
     </fill>
@@ -921,7 +944,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="15">
+  <borders count="23">
     <border>
       <left/>
       <right/>
@@ -931,42 +954,42 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </left>
       <right style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </right>
       <top style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </top>
       <bottom style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </left>
       <right style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </right>
       <top style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </top>
       <bottom/>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </left>
       <right/>
       <top style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </top>
       <bottom style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </bottom>
       <diagonal/>
     </border>
@@ -980,32 +1003,32 @@
     <border>
       <left/>
       <right style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </right>
       <top style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </top>
       <bottom style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </left>
       <right style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </right>
       <top/>
       <bottom style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </left>
       <right/>
       <top/>
@@ -1014,13 +1037,50 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="18"/>
+        <color indexed="10"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="10"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="17"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="10"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="17"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="10"/>
+      </right>
+      <top style="thin">
+        <color indexed="10"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="17"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="17"/>
       </left>
       <right style="thin">
-        <color indexed="18"/>
+        <color indexed="17"/>
       </right>
       <top style="thin">
-        <color indexed="18"/>
+        <color indexed="17"/>
       </top>
       <bottom style="thin">
         <color indexed="19"/>
@@ -1029,7 +1089,7 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="18"/>
+        <color indexed="17"/>
       </left>
       <right style="thin">
         <color indexed="19"/>
@@ -1038,7 +1098,7 @@
         <color indexed="19"/>
       </top>
       <bottom style="thin">
-        <color indexed="18"/>
+        <color indexed="17"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1047,43 +1107,43 @@
         <color indexed="19"/>
       </left>
       <right style="thin">
-        <color indexed="18"/>
+        <color indexed="17"/>
       </right>
       <top style="thin">
         <color indexed="19"/>
       </top>
       <bottom style="thin">
-        <color indexed="18"/>
+        <color indexed="17"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="18"/>
+        <color indexed="17"/>
       </left>
       <right style="thin">
-        <color indexed="18"/>
+        <color indexed="17"/>
       </right>
       <top style="thin">
         <color indexed="19"/>
       </top>
       <bottom style="thin">
-        <color indexed="18"/>
+        <color indexed="17"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="18"/>
+        <color indexed="17"/>
       </left>
       <right style="thin">
         <color indexed="19"/>
       </right>
       <top style="thin">
-        <color indexed="18"/>
+        <color indexed="17"/>
       </top>
       <bottom style="thin">
-        <color indexed="18"/>
+        <color indexed="17"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1092,28 +1152,103 @@
         <color indexed="19"/>
       </left>
       <right style="thin">
-        <color indexed="18"/>
+        <color indexed="17"/>
       </right>
       <top style="thin">
-        <color indexed="18"/>
+        <color indexed="17"/>
       </top>
       <bottom style="thin">
-        <color indexed="18"/>
+        <color indexed="17"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="18"/>
+        <color indexed="17"/>
       </left>
       <right style="thin">
-        <color indexed="18"/>
+        <color indexed="17"/>
       </right>
       <top style="thin">
-        <color indexed="18"/>
+        <color indexed="17"/>
       </top>
       <bottom style="thin">
-        <color indexed="18"/>
+        <color indexed="17"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="21"/>
+      </left>
+      <right style="thin">
+        <color indexed="21"/>
+      </right>
+      <top style="thin">
+        <color indexed="21"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="22"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="21"/>
+      </left>
+      <right style="thin">
+        <color indexed="22"/>
+      </right>
+      <top style="thin">
+        <color indexed="22"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="21"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="22"/>
+      </left>
+      <right style="thin">
+        <color indexed="21"/>
+      </right>
+      <top style="thin">
+        <color indexed="22"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="21"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="21"/>
+      </left>
+      <right style="thin">
+        <color indexed="22"/>
+      </right>
+      <top style="thin">
+        <color indexed="21"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="21"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="22"/>
+      </left>
+      <right style="thin">
+        <color indexed="21"/>
+      </right>
+      <top style="thin">
+        <color indexed="21"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="21"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1123,14 +1258,14 @@
       <alignment vertical="bottom"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="119">
+  <cellXfs count="131">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="3" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="49" fontId="3" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -1139,22 +1274,22 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="3" fontId="0" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="3" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="4" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="4" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="3" fontId="4" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="3" fontId="4" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
@@ -1166,52 +1301,52 @@
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="9" fontId="0" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="9" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="9" fontId="5" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="9" fontId="5" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="10" fontId="6" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="10" fontId="6" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="59" fontId="6" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="59" fontId="6" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="9" fontId="0" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="9" fontId="0" fillId="2" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="9" fontId="5" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="9" fontId="5" fillId="2" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="3" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="9" fontId="0" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="9" fontId="0" fillId="2" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="9" fontId="0" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="9" fontId="0" fillId="2" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="9" fontId="0" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="9" fontId="0" fillId="2" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="9" fontId="5" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="9" fontId="5" fillId="2" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="9" fontId="5" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="9" fontId="5" fillId="2" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="9" fontId="5" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="9" fontId="5" fillId="2" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="4" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="59" fontId="0" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="59" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="9" fontId="4" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="9" fontId="4" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
@@ -1220,49 +1355,49 @@
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="4" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="10" fontId="0" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="10" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="3" fontId="0" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="3" fontId="0" fillId="2" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="3" fontId="0" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="3" fontId="0" fillId="2" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="3" fontId="0" fillId="5" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="3" fontId="0" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="3" fontId="0" fillId="2" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="3" fontId="0" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="3" fontId="0" fillId="2" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="6" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -1274,10 +1409,10 @@
     <xf numFmtId="3" fontId="0" fillId="6" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="right" vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
@@ -1316,7 +1451,7 @@
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="60" fontId="0" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="60" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
@@ -1343,7 +1478,7 @@
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
@@ -1358,10 +1493,10 @@
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="1" fontId="0" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="1" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="1" fontId="0" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="1" fontId="0" fillId="2" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="6" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -1370,7 +1505,7 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="right" vertical="bottom"/>
     </xf>
-    <xf numFmtId="1" fontId="0" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="1" fontId="0" fillId="2" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
@@ -1394,7 +1529,7 @@
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="61" fontId="0" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="61" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
@@ -1406,7 +1541,85 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="10" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="10" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="11" fillId="2" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="9" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="10" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="8" borderId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="8" borderId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="9" borderId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="13" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="62" fontId="0" fillId="2" borderId="14" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="9" borderId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="16" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="17" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="17" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="17" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="62" fontId="7" fillId="2" borderId="17" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="63" fontId="0" fillId="2" borderId="17" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="17" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="17" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="2" borderId="17" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="62" fontId="0" fillId="2" borderId="17" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="17" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf numFmtId="62" fontId="7" fillId="2" borderId="17" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="2" borderId="17" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="2" borderId="17" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="17" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
@@ -1415,70 +1628,28 @@
     <xf numFmtId="0" fontId="2" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="8" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="13" borderId="18" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="8" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="13" borderId="18" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="14" borderId="19" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="9" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="14" borderId="20" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="14" borderId="21" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="11" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="14" borderId="22" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="62" fontId="0" borderId="11" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" borderId="21" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="9" borderId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" borderId="13" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="14" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="14" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" borderId="14" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="62" fontId="7" borderId="14" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="63" fontId="0" borderId="14" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" borderId="14" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" borderId="14" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="11" borderId="14" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="62" fontId="0" borderId="14" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" borderId="14" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf numFmtId="62" fontId="7" borderId="14" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" borderId="14" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" borderId="14" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" borderId="14" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="21" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
   </cellXfs>
@@ -1498,18 +1669,20 @@
       <rgbColor rgb="ffff00ff"/>
       <rgbColor rgb="ff00ffff"/>
       <rgbColor rgb="ff000000"/>
+      <rgbColor rgb="ffffffff"/>
       <rgbColor rgb="ffaaaaaa"/>
-      <rgbColor rgb="ffffffff"/>
       <rgbColor rgb="ffff0000"/>
       <rgbColor rgb="ff51a939"/>
       <rgbColor rgb="ffffff00"/>
       <rgbColor rgb="ffffc000"/>
       <rgbColor rgb="ff5b9bd5"/>
       <rgbColor rgb="ff598a38"/>
+      <rgbColor rgb="ffa5a5a5"/>
       <rgbColor rgb="ffbdc0bf"/>
+      <rgbColor rgb="ff3f3f3f"/>
+      <rgbColor rgb="ffdbdbdb"/>
       <rgbColor rgb="ffa5a5a5"/>
       <rgbColor rgb="ff3f3f3f"/>
-      <rgbColor rgb="ffdbdbdb"/>
     </indexedColors>
   </colors>
 </styleSheet>
@@ -1708,17 +1881,17 @@
         <a:solidFill>
           <a:srgbClr val="FFFFFF"/>
         </a:solidFill>
-        <a:ln w="12700" cap="flat">
+        <a:ln w="25400" cap="flat">
           <a:solidFill>
             <a:schemeClr val="accent1"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
+          <a:round/>
         </a:ln>
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -1746,10 +1919,10 @@
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="Calibri"/>
-            <a:ea typeface="Calibri"/>
-            <a:cs typeface="Calibri"/>
-            <a:sym typeface="Calibri"/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica Neue"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -1997,12 +2170,12 @@
     <a:lnDef>
       <a:spPr>
         <a:noFill/>
-        <a:ln w="12700" cap="flat">
+        <a:ln w="25400" cap="flat">
           <a:solidFill>
             <a:schemeClr val="accent1"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
+          <a:round/>
         </a:ln>
         <a:effectLst/>
         <a:sp3d/>
@@ -2289,7 +2462,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -2317,10 +2490,10 @@
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="Calibri"/>
-            <a:ea typeface="Calibri"/>
-            <a:cs typeface="Calibri"/>
-            <a:sym typeface="Calibri"/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica Neue"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -30656,7 +30829,7 @@
 
 <file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:N57"/>
+  <dimension ref="A1:N58"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -31259,40 +31432,40 @@
       <c r="N18" s="56"/>
     </row>
     <row r="19" ht="15" customHeight="1">
-      <c r="A19" t="s" s="5">
+      <c r="A19" t="s" s="53">
         <v>44</v>
       </c>
-      <c r="B19" t="s" s="5">
+      <c r="B19" t="s" s="53">
         <v>45</v>
       </c>
-      <c r="C19" s="6">
+      <c r="C19" s="54">
         <v>27010</v>
       </c>
-      <c r="D19" s="6">
+      <c r="D19" s="54">
         <v>7754</v>
       </c>
-      <c r="E19" s="6">
+      <c r="E19" s="54">
         <v>2691</v>
       </c>
-      <c r="F19" s="6">
+      <c r="F19" s="54">
         <v>844</v>
       </c>
-      <c r="G19" s="6">
+      <c r="G19" s="54">
         <v>1847</v>
       </c>
-      <c r="H19" s="6">
+      <c r="H19" s="54">
         <v>5063</v>
       </c>
-      <c r="I19" s="6">
+      <c r="I19" s="54">
         <v>4284</v>
       </c>
-      <c r="J19" s="6">
+      <c r="J19" s="54">
         <v>779</v>
       </c>
-      <c r="K19" s="7"/>
-      <c r="L19" s="7"/>
-      <c r="M19" s="7"/>
-      <c r="N19" s="7"/>
+      <c r="K19" s="56"/>
+      <c r="L19" s="56"/>
+      <c r="M19" s="56"/>
+      <c r="N19" s="56"/>
     </row>
     <row r="20" ht="15" customHeight="1" hidden="1">
       <c r="A20" t="s" s="5">
@@ -32020,47 +32193,51 @@
       <c r="M45" s="7"/>
       <c r="N45" s="7"/>
     </row>
-    <row r="46" ht="15" customHeight="1" hidden="1">
-      <c r="A46" t="s" s="5">
+    <row r="46" ht="15" customHeight="1">
+      <c r="A46" t="s" s="53">
         <v>94</v>
       </c>
-      <c r="B46" t="s" s="5">
+      <c r="B46" t="s" s="53">
         <v>95</v>
       </c>
-      <c r="C46" s="6"/>
-      <c r="D46" s="6"/>
-      <c r="E46" s="6"/>
-      <c r="F46" s="6"/>
-      <c r="G46" s="6"/>
-      <c r="H46" s="6"/>
-      <c r="I46" s="6"/>
-      <c r="J46" s="6"/>
-      <c r="K46" s="7"/>
-      <c r="L46" s="7"/>
-      <c r="M46" s="7"/>
-      <c r="N46" s="7"/>
-    </row>
-    <row r="47" ht="15" customHeight="1">
+      <c r="C46" s="54">
+        <v>121119</v>
+      </c>
+      <c r="D46" s="54">
+        <v>25822</v>
+      </c>
+      <c r="E46" s="54">
+        <v>19350</v>
+      </c>
+      <c r="F46" s="54"/>
+      <c r="G46" s="54"/>
+      <c r="H46" s="54">
+        <v>6472</v>
+      </c>
+      <c r="I46" s="54">
+        <v>4878</v>
+      </c>
+      <c r="J46" s="54">
+        <v>1594</v>
+      </c>
+      <c r="K46" s="56"/>
+      <c r="L46" s="56"/>
+      <c r="M46" s="56"/>
+      <c r="N46" s="56"/>
+    </row>
+    <row r="47" ht="15" customHeight="1" hidden="1">
       <c r="A47" t="s" s="5">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B47" t="s" s="5">
-        <v>97</v>
-      </c>
-      <c r="C47" s="6">
-        <v>5579</v>
-      </c>
-      <c r="D47" s="6">
-        <v>2652</v>
-      </c>
-      <c r="E47" s="6">
-        <v>1152</v>
-      </c>
+        <v>95</v>
+      </c>
+      <c r="C47" s="6"/>
+      <c r="D47" s="6"/>
+      <c r="E47" s="6"/>
       <c r="F47" s="6"/>
       <c r="G47" s="6"/>
-      <c r="H47" s="6">
-        <v>1500</v>
-      </c>
+      <c r="H47" s="6"/>
       <c r="I47" s="6"/>
       <c r="J47" s="6"/>
       <c r="K47" s="7"/>
@@ -32068,19 +32245,27 @@
       <c r="M47" s="7"/>
       <c r="N47" s="7"/>
     </row>
-    <row r="48" ht="15" customHeight="1" hidden="1">
+    <row r="48" ht="15" customHeight="1">
       <c r="A48" t="s" s="5">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B48" t="s" s="5">
-        <v>99</v>
-      </c>
-      <c r="C48" s="6"/>
-      <c r="D48" s="6"/>
-      <c r="E48" s="6"/>
+        <v>97</v>
+      </c>
+      <c r="C48" s="6">
+        <v>5579</v>
+      </c>
+      <c r="D48" s="6">
+        <v>2652</v>
+      </c>
+      <c r="E48" s="6">
+        <v>1152</v>
+      </c>
       <c r="F48" s="6"/>
       <c r="G48" s="6"/>
-      <c r="H48" s="6"/>
+      <c r="H48" s="6">
+        <v>1500</v>
+      </c>
       <c r="I48" s="6"/>
       <c r="J48" s="6"/>
       <c r="K48" s="7"/>
@@ -32088,29 +32273,19 @@
       <c r="M48" s="7"/>
       <c r="N48" s="7"/>
     </row>
-    <row r="49" ht="15" customHeight="1">
+    <row r="49" ht="15" customHeight="1" hidden="1">
       <c r="A49" t="s" s="5">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B49" t="s" s="5">
-        <v>101</v>
-      </c>
-      <c r="C49" s="8">
-        <v>1066</v>
-      </c>
-      <c r="D49" s="6">
-        <f>E49+H49</f>
-        <v>250</v>
-      </c>
-      <c r="E49" s="6">
-        <v>92</v>
-      </c>
+        <v>99</v>
+      </c>
+      <c r="C49" s="6"/>
+      <c r="D49" s="6"/>
+      <c r="E49" s="6"/>
       <c r="F49" s="6"/>
-      <c r="G49" s="7"/>
-      <c r="H49" s="6">
-        <f>27+131</f>
-        <v>158</v>
-      </c>
+      <c r="G49" s="6"/>
+      <c r="H49" s="6"/>
       <c r="I49" s="6"/>
       <c r="J49" s="6"/>
       <c r="K49" s="7"/>
@@ -32120,95 +32295,95 @@
     </row>
     <row r="50" ht="15" customHeight="1">
       <c r="A50" t="s" s="5">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B50" t="s" s="5">
-        <v>103</v>
-      </c>
-      <c r="C50" s="6">
-        <v>17330</v>
+        <v>101</v>
+      </c>
+      <c r="C50" s="8">
+        <v>1066</v>
       </c>
       <c r="D50" s="6">
-        <v>6054</v>
-      </c>
-      <c r="E50" s="6"/>
+        <f>E50+H50</f>
+        <v>250</v>
+      </c>
+      <c r="E50" s="6">
+        <v>92</v>
+      </c>
       <c r="F50" s="6"/>
-      <c r="G50" s="6"/>
+      <c r="G50" s="7"/>
       <c r="H50" s="6">
-        <v>6054</v>
-      </c>
-      <c r="I50" s="6">
-        <v>4064</v>
-      </c>
-      <c r="J50" s="6">
-        <v>1990</v>
-      </c>
+        <f>27+131</f>
+        <v>158</v>
+      </c>
+      <c r="I50" s="6"/>
+      <c r="J50" s="6"/>
       <c r="K50" s="7"/>
       <c r="L50" s="7"/>
       <c r="M50" s="7"/>
-      <c r="N50" s="6"/>
+      <c r="N50" s="7"/>
     </row>
     <row r="51" ht="15" customHeight="1">
       <c r="A51" t="s" s="5">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B51" t="s" s="5">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C51" s="6">
-        <v>23765</v>
+        <v>17330</v>
       </c>
       <c r="D51" s="6">
-        <v>12152</v>
-      </c>
-      <c r="E51" s="6">
-        <v>4676</v>
-      </c>
-      <c r="F51" s="6">
-        <v>2672</v>
-      </c>
-      <c r="G51" s="6">
-        <v>2004</v>
-      </c>
+        <v>6054</v>
+      </c>
+      <c r="E51" s="6"/>
+      <c r="F51" s="6"/>
+      <c r="G51" s="6"/>
       <c r="H51" s="6">
-        <v>7476</v>
+        <v>6054</v>
       </c>
       <c r="I51" s="6">
-        <v>3768</v>
+        <v>4064</v>
       </c>
       <c r="J51" s="6">
-        <v>3708</v>
+        <v>1990</v>
       </c>
       <c r="K51" s="7"/>
       <c r="L51" s="7"/>
       <c r="M51" s="7"/>
-      <c r="N51" s="7"/>
+      <c r="N51" s="6"/>
     </row>
     <row r="52" ht="15" customHeight="1">
       <c r="A52" t="s" s="5">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B52" t="s" s="5">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C52" s="6">
-        <v>6640</v>
+        <v>23765</v>
       </c>
       <c r="D52" s="6">
-        <v>865</v>
+        <v>12152</v>
       </c>
       <c r="E52" s="6">
-        <v>865</v>
+        <v>4676</v>
       </c>
       <c r="F52" s="6">
-        <v>65</v>
+        <v>2672</v>
       </c>
       <c r="G52" s="6">
-        <v>800</v>
-      </c>
-      <c r="H52" s="6"/>
-      <c r="I52" s="6"/>
-      <c r="J52" s="6"/>
+        <v>2004</v>
+      </c>
+      <c r="H52" s="6">
+        <v>7476</v>
+      </c>
+      <c r="I52" s="6">
+        <v>3768</v>
+      </c>
+      <c r="J52" s="6">
+        <v>3708</v>
+      </c>
       <c r="K52" s="7"/>
       <c r="L52" s="7"/>
       <c r="M52" s="7"/>
@@ -32216,51 +32391,65 @@
     </row>
     <row r="53" ht="15" customHeight="1">
       <c r="A53" t="s" s="5">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B53" t="s" s="5">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C53" s="6">
-        <v>2364</v>
+        <v>6640</v>
       </c>
       <c r="D53" s="6">
-        <v>681</v>
+        <v>865</v>
       </c>
       <c r="E53" s="6">
-        <v>482</v>
+        <v>865</v>
       </c>
       <c r="F53" s="6">
-        <v>24</v>
+        <v>65</v>
       </c>
       <c r="G53" s="6">
-        <v>458</v>
-      </c>
-      <c r="H53" s="6">
-        <v>199</v>
-      </c>
-      <c r="I53" s="6">
-        <v>72</v>
-      </c>
-      <c r="J53" s="6">
-        <v>127</v>
-      </c>
+        <v>800</v>
+      </c>
+      <c r="H53" s="6"/>
+      <c r="I53" s="6"/>
+      <c r="J53" s="6"/>
       <c r="K53" s="7"/>
       <c r="L53" s="7"/>
       <c r="M53" s="7"/>
       <c r="N53" s="7"/>
     </row>
     <row r="54" ht="15" customHeight="1">
-      <c r="A54" s="7"/>
-      <c r="B54" s="7"/>
-      <c r="C54" s="7"/>
-      <c r="D54" s="7"/>
-      <c r="E54" s="7"/>
-      <c r="F54" s="7"/>
-      <c r="G54" s="7"/>
-      <c r="H54" s="7"/>
-      <c r="I54" s="7"/>
-      <c r="J54" s="7"/>
+      <c r="A54" t="s" s="5">
+        <v>108</v>
+      </c>
+      <c r="B54" t="s" s="5">
+        <v>109</v>
+      </c>
+      <c r="C54" s="6">
+        <v>2364</v>
+      </c>
+      <c r="D54" s="6">
+        <v>681</v>
+      </c>
+      <c r="E54" s="6">
+        <v>482</v>
+      </c>
+      <c r="F54" s="6">
+        <v>24</v>
+      </c>
+      <c r="G54" s="6">
+        <v>458</v>
+      </c>
+      <c r="H54" s="6">
+        <v>199</v>
+      </c>
+      <c r="I54" s="6">
+        <v>72</v>
+      </c>
+      <c r="J54" s="6">
+        <v>127</v>
+      </c>
       <c r="K54" s="7"/>
       <c r="L54" s="7"/>
       <c r="M54" s="7"/>
@@ -32268,103 +32457,119 @@
     </row>
     <row r="55" ht="15" customHeight="1">
       <c r="A55" s="7"/>
-      <c r="B55" t="s" s="9">
-        <v>110</v>
-      </c>
-      <c r="C55" s="10">
-        <f>SUM(C2:C53)</f>
-        <v>779893</v>
-      </c>
-      <c r="D55" s="10">
-        <f>SUM(D2:D53)</f>
-        <v>155945</v>
-      </c>
-      <c r="E55" s="10">
-        <f>SUM(E2:E53)</f>
-        <v>141942</v>
-      </c>
-      <c r="F55" s="10">
-        <f>SUM(F2:F53)+E22+E23+E31+E43+E47+E49</f>
-        <v>45665</v>
-      </c>
-      <c r="G55" s="10">
-        <f>SUM(G2:G53)</f>
-        <v>25258</v>
-      </c>
-      <c r="H55" s="10">
-        <f>SUM(H2:H53)</f>
-        <v>85007</v>
-      </c>
-      <c r="I55" s="10">
-        <f>SUM(I2:I53)+H23+H31+H43+H47+H49</f>
-        <v>61391</v>
-      </c>
-      <c r="J55" s="10">
-        <f>SUM(J2:J53)</f>
-        <v>23595</v>
-      </c>
+      <c r="B55" s="7"/>
+      <c r="C55" s="7"/>
+      <c r="D55" s="7"/>
+      <c r="E55" s="7"/>
+      <c r="F55" s="7"/>
+      <c r="G55" s="7"/>
+      <c r="H55" s="7"/>
+      <c r="I55" s="7"/>
+      <c r="J55" s="7"/>
       <c r="K55" s="7"/>
-      <c r="L55" s="6"/>
+      <c r="L55" s="7"/>
       <c r="M55" s="7"/>
       <c r="N55" s="7"/>
     </row>
     <row r="56" ht="15" customHeight="1">
       <c r="A56" s="7"/>
-      <c r="B56" s="7"/>
-      <c r="C56" s="7"/>
-      <c r="D56" s="7"/>
-      <c r="E56" s="7"/>
-      <c r="F56" s="7"/>
-      <c r="G56" s="7"/>
-      <c r="H56" s="7"/>
-      <c r="I56" s="7"/>
-      <c r="J56" s="7"/>
+      <c r="B56" t="s" s="9">
+        <v>110</v>
+      </c>
+      <c r="C56" s="10">
+        <f>SUM(C2:C54)</f>
+        <v>901012</v>
+      </c>
+      <c r="D56" s="10">
+        <f>SUM(D2:D54)</f>
+        <v>181767</v>
+      </c>
+      <c r="E56" s="10">
+        <f>SUM(E2:E54)</f>
+        <v>161292</v>
+      </c>
+      <c r="F56" s="10">
+        <f>SUM(F2:F54)+E22+E23+E31+E43+E48+E50</f>
+        <v>45665</v>
+      </c>
+      <c r="G56" s="10">
+        <f>SUM(G2:G54)</f>
+        <v>25258</v>
+      </c>
+      <c r="H56" s="10">
+        <f>SUM(H2:H54)</f>
+        <v>91479</v>
+      </c>
+      <c r="I56" s="10">
+        <f>SUM(I2:I54)+H23+H31+H43+H48+H50</f>
+        <v>66269</v>
+      </c>
+      <c r="J56" s="10">
+        <f>SUM(J2:J54)</f>
+        <v>25189</v>
+      </c>
       <c r="K56" s="7"/>
-      <c r="L56" s="7"/>
+      <c r="L56" s="6"/>
       <c r="M56" s="7"/>
       <c r="N56" s="7"/>
     </row>
     <row r="57" ht="15" customHeight="1">
       <c r="A57" s="7"/>
-      <c r="B57" t="s" s="5">
-        <v>140</v>
-      </c>
-      <c r="C57" s="8">
-        <f>COUNTIF(C2:C53,"&gt;0")</f>
-        <v>41</v>
-      </c>
-      <c r="D57" s="8">
-        <f>COUNTIF(D2:D53,"&gt;0")</f>
-        <v>36</v>
-      </c>
-      <c r="E57" s="8">
-        <f>COUNTIF(E2:E53,"&gt;0")</f>
-        <v>31</v>
-      </c>
-      <c r="F57" s="8">
-        <f>COUNTIF(F2:F53,"&gt;0")</f>
-        <v>22</v>
-      </c>
-      <c r="G57" s="8">
-        <f>COUNTIF(G2:G53,"&gt;0")</f>
-        <v>25</v>
-      </c>
-      <c r="H57" s="8">
-        <f>COUNTIF(H2:H53,"&gt;0")</f>
-        <v>34</v>
-      </c>
-      <c r="I57" s="8">
-        <f>COUNTIF(I2:I53,"&gt;0")</f>
-        <v>26</v>
-      </c>
-      <c r="J57" s="8">
-        <f>COUNTIF(J2:J53,"&gt;0")</f>
-        <v>29</v>
-      </c>
+      <c r="B57" s="7"/>
+      <c r="C57" s="7"/>
+      <c r="D57" s="7"/>
+      <c r="E57" s="7"/>
+      <c r="F57" s="7"/>
+      <c r="G57" s="7"/>
+      <c r="H57" s="7"/>
+      <c r="I57" s="7"/>
+      <c r="J57" s="7"/>
       <c r="K57" s="7"/>
       <c r="L57" s="7"/>
       <c r="M57" s="7"/>
       <c r="N57" s="7"/>
+    </row>
+    <row r="58" ht="15" customHeight="1">
+      <c r="A58" s="7"/>
+      <c r="B58" t="s" s="5">
+        <v>140</v>
+      </c>
+      <c r="C58" s="8">
+        <f>COUNTIF(C2:C54,"&gt;0")</f>
+        <v>42</v>
+      </c>
+      <c r="D58" s="8">
+        <f>COUNTIF(D2:D54,"&gt;0")</f>
+        <v>37</v>
+      </c>
+      <c r="E58" s="8">
+        <f>COUNTIF(E2:E54,"&gt;0")</f>
+        <v>32</v>
+      </c>
+      <c r="F58" s="8">
+        <f>COUNTIF(F2:F54,"&gt;0")</f>
+        <v>22</v>
+      </c>
+      <c r="G58" s="8">
+        <f>COUNTIF(G2:G54,"&gt;0")</f>
+        <v>25</v>
+      </c>
+      <c r="H58" s="8">
+        <f>COUNTIF(H2:H54,"&gt;0")</f>
+        <v>35</v>
+      </c>
+      <c r="I58" s="8">
+        <f>COUNTIF(I2:I54,"&gt;0")</f>
+        <v>27</v>
+      </c>
+      <c r="J58" s="8">
+        <f>COUNTIF(J2:J54,"&gt;0")</f>
+        <v>30</v>
+      </c>
+      <c r="K58" s="7"/>
+      <c r="L58" s="7"/>
+      <c r="M58" s="7"/>
+      <c r="N58" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -37878,11 +38083,9 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A2:I52"/>
+  <dimension ref="A1:I52"/>
   <sheetViews>
-    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1">
-      <pane topLeftCell="B3" xSplit="1" ySplit="2" activePane="bottomRight" state="frozen"/>
-    </sheetView>
+    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="14.75" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
@@ -37902,941 +38105,1337 @@
       <c r="A1" t="s" s="96">
         <v>197</v>
       </c>
-      <c r="B1" s="96"/>
-      <c r="C1" s="96"/>
-      <c r="D1" s="96"/>
-      <c r="E1" s="96"/>
-      <c r="F1" s="96"/>
-      <c r="G1" s="96"/>
-      <c r="H1" s="96"/>
-      <c r="I1" s="96"/>
+      <c r="B1" s="97"/>
+      <c r="C1" s="97"/>
+      <c r="D1" s="97"/>
+      <c r="E1" s="97"/>
+      <c r="F1" s="97"/>
+      <c r="G1" s="97"/>
+      <c r="H1" s="97"/>
+      <c r="I1" s="98"/>
     </row>
     <row r="2" ht="14.55" customHeight="1">
-      <c r="A2" t="s" s="97">
+      <c r="A2" t="s" s="99">
         <v>0</v>
       </c>
-      <c r="B2" t="s" s="97">
+      <c r="B2" t="s" s="99">
         <v>1</v>
       </c>
-      <c r="C2" t="s" s="98">
+      <c r="C2" t="s" s="100">
         <v>198</v>
       </c>
-      <c r="D2" t="s" s="98">
+      <c r="D2" t="s" s="100">
         <v>199</v>
       </c>
-      <c r="E2" t="s" s="98">
+      <c r="E2" t="s" s="100">
         <v>200</v>
       </c>
-      <c r="F2" t="s" s="98">
+      <c r="F2" t="s" s="100">
         <v>201</v>
       </c>
-      <c r="G2" t="s" s="98">
+      <c r="G2" t="s" s="100">
         <v>202</v>
       </c>
-      <c r="H2" t="s" s="98">
+      <c r="H2" t="s" s="100">
         <v>203</v>
       </c>
-      <c r="I2" t="s" s="98">
+      <c r="I2" t="s" s="100">
         <v>149</v>
       </c>
     </row>
     <row r="3" ht="14.55" customHeight="1">
-      <c r="A3" t="s" s="99">
+      <c r="A3" t="s" s="101">
         <v>10</v>
       </c>
-      <c r="B3" t="s" s="100">
+      <c r="B3" t="s" s="102">
         <v>11</v>
       </c>
-      <c r="C3" s="101"/>
-      <c r="D3" s="101"/>
-      <c r="E3" s="101"/>
-      <c r="F3" s="101"/>
-      <c r="G3" s="102">
+      <c r="C3" s="103"/>
+      <c r="D3" s="103"/>
+      <c r="E3" s="103"/>
+      <c r="F3" s="103"/>
+      <c r="G3" s="104">
         <v>175.84</v>
       </c>
-      <c r="H3" s="101"/>
-      <c r="I3" s="101"/>
+      <c r="H3" s="103"/>
+      <c r="I3" s="103"/>
     </row>
     <row r="4" ht="15.95" customHeight="1">
-      <c r="A4" t="s" s="103">
+      <c r="A4" t="s" s="105">
         <v>12</v>
       </c>
-      <c r="B4" t="s" s="104">
+      <c r="B4" t="s" s="106">
         <v>13</v>
       </c>
-      <c r="C4" s="105"/>
-      <c r="D4" s="106">
+      <c r="C4" s="107"/>
+      <c r="D4" s="108">
         <v>45</v>
       </c>
-      <c r="E4" s="106">
+      <c r="E4" s="108">
         <v>45</v>
       </c>
-      <c r="F4" t="s" s="107">
+      <c r="F4" t="s" s="109">
         <v>204</v>
       </c>
-      <c r="G4" s="108">
+      <c r="G4" s="110">
         <v>72.28</v>
       </c>
-      <c r="H4" s="105"/>
-      <c r="I4" s="105"/>
+      <c r="H4" s="107"/>
+      <c r="I4" s="107"/>
     </row>
     <row r="5" ht="14.35" customHeight="1">
-      <c r="A5" t="s" s="103">
+      <c r="A5" t="s" s="105">
         <v>14</v>
       </c>
-      <c r="B5" t="s" s="104">
+      <c r="B5" t="s" s="106">
         <v>15</v>
       </c>
-      <c r="C5" s="105"/>
-      <c r="D5" s="105"/>
-      <c r="E5" s="105"/>
-      <c r="F5" s="105"/>
-      <c r="G5" s="105"/>
-      <c r="H5" s="105"/>
-      <c r="I5" s="105"/>
+      <c r="C5" s="107"/>
+      <c r="D5" s="107"/>
+      <c r="E5" s="107"/>
+      <c r="F5" s="107"/>
+      <c r="G5" s="107"/>
+      <c r="H5" s="107"/>
+      <c r="I5" s="107"/>
     </row>
     <row r="6" ht="26.35" customHeight="1">
-      <c r="A6" t="s" s="103">
+      <c r="A6" t="s" s="105">
         <v>16</v>
       </c>
-      <c r="B6" t="s" s="104">
+      <c r="B6" t="s" s="106">
         <v>17</v>
       </c>
-      <c r="C6" s="109">
+      <c r="C6" s="111">
         <v>1061.7</v>
       </c>
-      <c r="D6" s="110">
+      <c r="D6" s="112">
         <v>686.6</v>
       </c>
-      <c r="E6" s="111">
+      <c r="E6" s="113">
         <v>238.5</v>
       </c>
-      <c r="F6" t="s" s="112">
+      <c r="F6" t="s" s="114">
         <v>204</v>
       </c>
-      <c r="G6" s="113">
+      <c r="G6" s="115">
         <v>71.48999999999999</v>
       </c>
-      <c r="H6" s="113">
+      <c r="H6" s="115">
         <v>4.91</v>
       </c>
-      <c r="I6" t="s" s="114">
+      <c r="I6" t="s" s="116">
         <v>205</v>
       </c>
     </row>
     <row r="7" ht="14.35" customHeight="1">
-      <c r="A7" t="s" s="103">
+      <c r="A7" t="s" s="105">
         <v>18</v>
       </c>
-      <c r="B7" t="s" s="104">
+      <c r="B7" t="s" s="106">
         <v>19</v>
       </c>
-      <c r="C7" s="105"/>
-      <c r="D7" s="105"/>
-      <c r="E7" s="105"/>
-      <c r="F7" s="105"/>
-      <c r="G7" s="105"/>
-      <c r="H7" s="105"/>
-      <c r="I7" s="105"/>
+      <c r="C7" s="107"/>
+      <c r="D7" s="107"/>
+      <c r="E7" s="107"/>
+      <c r="F7" s="107"/>
+      <c r="G7" s="107"/>
+      <c r="H7" s="107"/>
+      <c r="I7" s="107"/>
     </row>
     <row r="8" ht="14.35" customHeight="1">
-      <c r="A8" t="s" s="103">
+      <c r="A8" t="s" s="105">
         <v>20</v>
       </c>
-      <c r="B8" t="s" s="104">
+      <c r="B8" t="s" s="106">
         <v>21</v>
       </c>
-      <c r="C8" s="106">
+      <c r="C8" s="108">
         <v>953</v>
       </c>
-      <c r="D8" s="106">
+      <c r="D8" s="108">
         <v>1170</v>
       </c>
-      <c r="E8" s="106">
+      <c r="E8" s="108">
         <v>511</v>
       </c>
-      <c r="F8" t="s" s="107">
+      <c r="F8" t="s" s="109">
         <v>204</v>
       </c>
-      <c r="G8" s="105"/>
-      <c r="H8" s="105"/>
-      <c r="I8" s="105"/>
+      <c r="G8" s="107"/>
+      <c r="H8" s="107"/>
+      <c r="I8" s="107"/>
     </row>
     <row r="9" ht="14.35" customHeight="1">
-      <c r="A9" t="s" s="103">
+      <c r="A9" t="s" s="105">
         <v>22</v>
       </c>
-      <c r="B9" t="s" s="104">
+      <c r="B9" t="s" s="106">
         <v>23</v>
       </c>
-      <c r="C9" s="105"/>
-      <c r="D9" s="105"/>
-      <c r="E9" s="105"/>
-      <c r="F9" s="105"/>
-      <c r="G9" s="113">
+      <c r="C9" s="107"/>
+      <c r="D9" s="107"/>
+      <c r="E9" s="107"/>
+      <c r="F9" s="107"/>
+      <c r="G9" s="115">
         <v>131.15</v>
       </c>
-      <c r="H9" s="105"/>
-      <c r="I9" s="105"/>
+      <c r="H9" s="107"/>
+      <c r="I9" s="107"/>
     </row>
     <row r="10" ht="14.35" customHeight="1">
-      <c r="A10" t="s" s="103">
+      <c r="A10" t="s" s="105">
         <v>24</v>
       </c>
-      <c r="B10" t="s" s="104">
+      <c r="B10" t="s" s="106">
         <v>25</v>
       </c>
-      <c r="C10" s="105"/>
-      <c r="D10" s="105"/>
-      <c r="E10" s="105"/>
-      <c r="F10" s="105"/>
-      <c r="G10" s="105"/>
-      <c r="H10" s="105"/>
-      <c r="I10" s="105"/>
+      <c r="C10" s="107"/>
+      <c r="D10" s="107"/>
+      <c r="E10" s="107"/>
+      <c r="F10" s="107"/>
+      <c r="G10" s="107"/>
+      <c r="H10" s="107"/>
+      <c r="I10" s="107"/>
     </row>
     <row r="11" ht="14.35" customHeight="1">
-      <c r="A11" t="s" s="103">
+      <c r="A11" t="s" s="105">
         <v>26</v>
       </c>
-      <c r="B11" t="s" s="104">
+      <c r="B11" t="s" s="106">
         <v>27</v>
       </c>
-      <c r="C11" s="105"/>
-      <c r="D11" s="105"/>
-      <c r="E11" s="105"/>
-      <c r="F11" s="105"/>
-      <c r="G11" s="105"/>
-      <c r="H11" s="105"/>
-      <c r="I11" s="105"/>
+      <c r="C11" s="107"/>
+      <c r="D11" s="107"/>
+      <c r="E11" s="107"/>
+      <c r="F11" s="107"/>
+      <c r="G11" s="107"/>
+      <c r="H11" s="107"/>
+      <c r="I11" s="107"/>
     </row>
     <row r="12" ht="14.35" customHeight="1">
-      <c r="A12" t="s" s="103">
+      <c r="A12" t="s" s="105">
         <v>28</v>
       </c>
-      <c r="B12" t="s" s="104">
+      <c r="B12" t="s" s="106">
         <v>29</v>
       </c>
-      <c r="C12" s="105"/>
-      <c r="D12" s="105"/>
-      <c r="E12" s="105"/>
-      <c r="F12" s="105"/>
-      <c r="G12" s="105"/>
-      <c r="H12" s="105"/>
-      <c r="I12" s="105"/>
+      <c r="C12" s="107"/>
+      <c r="D12" s="107"/>
+      <c r="E12" s="107"/>
+      <c r="F12" s="107"/>
+      <c r="G12" s="107"/>
+      <c r="H12" s="107"/>
+      <c r="I12" s="107"/>
     </row>
     <row r="13" ht="14.35" customHeight="1">
-      <c r="A13" t="s" s="103">
+      <c r="A13" t="s" s="105">
         <v>30</v>
       </c>
-      <c r="B13" t="s" s="104">
+      <c r="B13" t="s" s="106">
         <v>31</v>
       </c>
-      <c r="C13" s="105"/>
-      <c r="D13" s="105"/>
-      <c r="E13" s="105"/>
-      <c r="F13" s="105"/>
-      <c r="G13" s="105"/>
-      <c r="H13" s="105"/>
-      <c r="I13" s="105"/>
+      <c r="C13" s="107"/>
+      <c r="D13" s="107"/>
+      <c r="E13" s="107"/>
+      <c r="F13" s="107"/>
+      <c r="G13" s="107"/>
+      <c r="H13" s="107"/>
+      <c r="I13" s="107"/>
     </row>
     <row r="14" ht="14.35" customHeight="1">
-      <c r="A14" t="s" s="103">
+      <c r="A14" t="s" s="105">
         <v>32</v>
       </c>
-      <c r="B14" t="s" s="104">
+      <c r="B14" t="s" s="106">
         <v>33</v>
       </c>
-      <c r="C14" s="105"/>
-      <c r="D14" s="105"/>
-      <c r="E14" s="105"/>
-      <c r="F14" s="105"/>
-      <c r="G14" s="105"/>
-      <c r="H14" s="105"/>
-      <c r="I14" s="105"/>
+      <c r="C14" s="107"/>
+      <c r="D14" s="107"/>
+      <c r="E14" s="107"/>
+      <c r="F14" s="107"/>
+      <c r="G14" s="107"/>
+      <c r="H14" s="107"/>
+      <c r="I14" s="107"/>
     </row>
     <row r="15" ht="15.95" customHeight="1">
-      <c r="A15" t="s" s="103">
+      <c r="A15" t="s" s="105">
         <v>34</v>
       </c>
-      <c r="B15" t="s" s="104">
+      <c r="B15" t="s" s="106">
         <v>35</v>
       </c>
-      <c r="C15" s="106">
+      <c r="C15" s="108">
         <v>61</v>
       </c>
-      <c r="D15" s="106">
+      <c r="D15" s="108">
         <v>24</v>
       </c>
-      <c r="E15" s="106">
+      <c r="E15" s="108">
         <v>25</v>
       </c>
-      <c r="F15" t="s" s="107">
+      <c r="F15" t="s" s="109">
         <v>206</v>
       </c>
-      <c r="G15" s="115">
+      <c r="G15" s="117">
         <v>76.31999999999999</v>
       </c>
-      <c r="H15" s="113">
+      <c r="H15" s="115">
         <v>32.14</v>
       </c>
-      <c r="I15" s="105"/>
+      <c r="I15" s="107"/>
     </row>
     <row r="16" ht="14.35" customHeight="1">
-      <c r="A16" t="s" s="103">
+      <c r="A16" t="s" s="105">
         <v>36</v>
       </c>
-      <c r="B16" t="s" s="104">
+      <c r="B16" t="s" s="106">
         <v>37</v>
       </c>
-      <c r="C16" s="106">
+      <c r="C16" s="108">
         <v>26.7</v>
       </c>
-      <c r="D16" s="105"/>
-      <c r="E16" s="106">
+      <c r="D16" s="107"/>
+      <c r="E16" s="108">
         <v>7.4</v>
       </c>
-      <c r="F16" t="s" s="107">
+      <c r="F16" t="s" s="109">
         <v>206</v>
       </c>
-      <c r="G16" s="113">
+      <c r="G16" s="115">
         <v>94.14</v>
       </c>
-      <c r="H16" s="113">
+      <c r="H16" s="115">
         <v>24.71</v>
       </c>
-      <c r="I16" t="s" s="107">
+      <c r="I16" t="s" s="109">
         <v>207</v>
       </c>
     </row>
     <row r="17" ht="14.35" customHeight="1">
-      <c r="A17" t="s" s="103">
+      <c r="A17" t="s" s="105">
         <v>38</v>
       </c>
-      <c r="B17" t="s" s="104">
+      <c r="B17" t="s" s="106">
         <v>39</v>
       </c>
-      <c r="C17" s="105"/>
-      <c r="D17" s="105"/>
-      <c r="E17" s="105"/>
-      <c r="F17" s="105"/>
-      <c r="G17" s="105"/>
-      <c r="H17" s="105"/>
-      <c r="I17" s="105"/>
+      <c r="C17" s="107"/>
+      <c r="D17" s="107"/>
+      <c r="E17" s="107"/>
+      <c r="F17" s="107"/>
+      <c r="G17" s="107"/>
+      <c r="H17" s="107"/>
+      <c r="I17" s="107"/>
     </row>
     <row r="18" ht="15.95" customHeight="1">
-      <c r="A18" t="s" s="103">
+      <c r="A18" t="s" s="105">
         <v>40</v>
       </c>
-      <c r="B18" t="s" s="104">
+      <c r="B18" t="s" s="106">
         <v>41</v>
       </c>
-      <c r="C18" s="106">
+      <c r="C18" s="108">
         <v>37.86</v>
       </c>
-      <c r="D18" s="106">
+      <c r="D18" s="108">
         <v>12.43</v>
       </c>
-      <c r="E18" s="106">
+      <c r="E18" s="108">
         <v>16.74</v>
       </c>
-      <c r="F18" t="s" s="107">
+      <c r="F18" t="s" s="109">
         <v>206</v>
       </c>
-      <c r="G18" t="s" s="116">
+      <c r="G18" t="s" s="118">
         <v>208</v>
       </c>
-      <c r="H18" s="105"/>
-      <c r="I18" t="s" s="107">
+      <c r="H18" s="107"/>
+      <c r="I18" t="s" s="109">
         <v>209</v>
       </c>
     </row>
     <row r="19" ht="14.35" customHeight="1">
-      <c r="A19" t="s" s="103">
+      <c r="A19" t="s" s="105">
         <v>42</v>
       </c>
-      <c r="B19" t="s" s="104">
+      <c r="B19" t="s" s="106">
         <v>43</v>
       </c>
-      <c r="C19" s="105"/>
-      <c r="D19" s="105"/>
-      <c r="E19" s="105"/>
-      <c r="F19" s="105"/>
-      <c r="G19" s="105"/>
-      <c r="H19" s="105"/>
-      <c r="I19" s="105"/>
+      <c r="C19" s="107"/>
+      <c r="D19" s="107"/>
+      <c r="E19" s="107"/>
+      <c r="F19" s="107"/>
+      <c r="G19" s="107"/>
+      <c r="H19" s="107"/>
+      <c r="I19" s="107"/>
     </row>
     <row r="20" ht="15.95" customHeight="1">
-      <c r="A20" t="s" s="103">
+      <c r="A20" t="s" s="105">
         <v>44</v>
       </c>
-      <c r="B20" t="s" s="104">
+      <c r="B20" t="s" s="106">
         <v>45</v>
       </c>
-      <c r="C20" s="106">
+      <c r="C20" s="108">
         <v>6.2</v>
       </c>
-      <c r="D20" s="106">
+      <c r="D20" s="108">
         <v>4.9</v>
       </c>
-      <c r="E20" s="106">
+      <c r="E20" s="108">
         <v>4.89</v>
       </c>
-      <c r="F20" t="s" s="107">
+      <c r="F20" t="s" s="109">
         <v>210</v>
       </c>
-      <c r="G20" t="s" s="117">
+      <c r="G20" t="s" s="119">
         <v>211</v>
       </c>
-      <c r="H20" t="s" s="107">
+      <c r="H20" t="s" s="109">
         <v>212</v>
       </c>
-      <c r="I20" t="s" s="107">
+      <c r="I20" t="s" s="109">
         <v>213</v>
       </c>
     </row>
     <row r="21" ht="14.35" customHeight="1">
-      <c r="A21" t="s" s="103">
+      <c r="A21" t="s" s="105">
         <v>46</v>
       </c>
-      <c r="B21" t="s" s="104">
+      <c r="B21" t="s" s="106">
         <v>47</v>
       </c>
-      <c r="C21" s="105"/>
-      <c r="D21" s="105"/>
-      <c r="E21" s="105"/>
-      <c r="F21" s="105"/>
-      <c r="G21" s="105"/>
-      <c r="H21" s="105"/>
-      <c r="I21" s="105"/>
+      <c r="C21" s="107"/>
+      <c r="D21" s="107"/>
+      <c r="E21" s="107"/>
+      <c r="F21" s="107"/>
+      <c r="G21" s="107"/>
+      <c r="H21" s="107"/>
+      <c r="I21" s="107"/>
     </row>
     <row r="22" ht="26.35" customHeight="1">
-      <c r="A22" t="s" s="103">
+      <c r="A22" t="s" s="105">
         <v>48</v>
       </c>
-      <c r="B22" t="s" s="104">
+      <c r="B22" t="s" s="106">
         <v>49</v>
       </c>
-      <c r="C22" s="105"/>
-      <c r="D22" s="105"/>
-      <c r="E22" s="105"/>
-      <c r="F22" s="105"/>
-      <c r="G22" s="113">
+      <c r="C22" s="107"/>
+      <c r="D22" s="107"/>
+      <c r="E22" s="107"/>
+      <c r="F22" s="107"/>
+      <c r="G22" s="115">
         <v>123.33</v>
       </c>
-      <c r="H22" s="113">
+      <c r="H22" s="115">
         <v>6.36</v>
       </c>
-      <c r="I22" t="s" s="114">
+      <c r="I22" t="s" s="116">
         <v>214</v>
       </c>
     </row>
     <row r="23" ht="14.35" customHeight="1">
-      <c r="A23" t="s" s="103">
+      <c r="A23" t="s" s="105">
         <v>50</v>
       </c>
-      <c r="B23" t="s" s="104">
+      <c r="B23" t="s" s="106">
         <v>51</v>
       </c>
-      <c r="C23" s="105"/>
-      <c r="D23" s="105"/>
-      <c r="E23" s="105"/>
-      <c r="F23" s="105"/>
-      <c r="G23" s="113">
+      <c r="C23" s="107"/>
+      <c r="D23" s="107"/>
+      <c r="E23" s="107"/>
+      <c r="F23" s="107"/>
+      <c r="G23" s="115">
         <v>151</v>
       </c>
-      <c r="H23" s="105"/>
-      <c r="I23" t="s" s="107">
+      <c r="H23" s="107"/>
+      <c r="I23" t="s" s="109">
         <v>215</v>
       </c>
     </row>
     <row r="24" ht="14.35" customHeight="1">
-      <c r="A24" t="s" s="103">
+      <c r="A24" t="s" s="105">
         <v>52</v>
       </c>
-      <c r="B24" t="s" s="104">
+      <c r="B24" t="s" s="106">
         <v>53</v>
       </c>
-      <c r="C24" s="105"/>
-      <c r="D24" s="105"/>
-      <c r="E24" s="105"/>
-      <c r="F24" s="105"/>
-      <c r="G24" s="105"/>
-      <c r="H24" s="105"/>
-      <c r="I24" s="105"/>
+      <c r="C24" s="107"/>
+      <c r="D24" s="107"/>
+      <c r="E24" s="107"/>
+      <c r="F24" s="107"/>
+      <c r="G24" s="107"/>
+      <c r="H24" s="107"/>
+      <c r="I24" s="107"/>
     </row>
     <row r="25" ht="14.35" customHeight="1">
-      <c r="A25" t="s" s="103">
+      <c r="A25" t="s" s="105">
         <v>54</v>
       </c>
-      <c r="B25" t="s" s="104">
+      <c r="B25" t="s" s="106">
         <v>55</v>
       </c>
-      <c r="C25" s="105"/>
-      <c r="D25" s="105"/>
-      <c r="E25" s="105"/>
-      <c r="F25" s="105"/>
-      <c r="G25" s="105"/>
-      <c r="H25" s="105"/>
-      <c r="I25" s="105"/>
+      <c r="C25" s="107"/>
+      <c r="D25" s="107"/>
+      <c r="E25" s="107"/>
+      <c r="F25" s="107"/>
+      <c r="G25" s="107"/>
+      <c r="H25" s="107"/>
+      <c r="I25" s="107"/>
     </row>
     <row r="26" ht="15.95" customHeight="1">
-      <c r="A26" t="s" s="103">
+      <c r="A26" t="s" s="105">
         <v>56</v>
       </c>
-      <c r="B26" t="s" s="104">
+      <c r="B26" t="s" s="106">
         <v>57</v>
       </c>
-      <c r="C26" s="106">
+      <c r="C26" s="108">
         <v>4.9</v>
       </c>
-      <c r="D26" s="106">
+      <c r="D26" s="108">
         <v>2.1</v>
       </c>
-      <c r="E26" s="106">
+      <c r="E26" s="108">
         <v>1.4</v>
       </c>
-      <c r="F26" t="s" s="107">
+      <c r="F26" t="s" s="109">
         <v>210</v>
       </c>
-      <c r="G26" t="s" s="117">
+      <c r="G26" t="s" s="119">
         <v>216</v>
       </c>
-      <c r="H26" t="s" s="117">
+      <c r="H26" t="s" s="119">
         <v>217</v>
       </c>
-      <c r="I26" s="118"/>
+      <c r="I26" s="120"/>
     </row>
     <row r="27" ht="14.35" customHeight="1">
-      <c r="A27" t="s" s="103">
+      <c r="A27" t="s" s="105">
         <v>58</v>
       </c>
-      <c r="B27" t="s" s="104">
+      <c r="B27" t="s" s="106">
         <v>59</v>
       </c>
-      <c r="C27" s="105"/>
-      <c r="D27" s="105"/>
-      <c r="E27" s="105"/>
-      <c r="F27" s="105"/>
-      <c r="G27" s="105"/>
-      <c r="H27" s="105"/>
-      <c r="I27" s="105"/>
+      <c r="C27" s="107"/>
+      <c r="D27" s="107"/>
+      <c r="E27" s="107"/>
+      <c r="F27" s="107"/>
+      <c r="G27" s="107"/>
+      <c r="H27" s="107"/>
+      <c r="I27" s="107"/>
     </row>
     <row r="28" ht="14.35" customHeight="1">
-      <c r="A28" t="s" s="103">
+      <c r="A28" t="s" s="105">
         <v>60</v>
       </c>
-      <c r="B28" t="s" s="104">
+      <c r="B28" t="s" s="106">
         <v>61</v>
       </c>
-      <c r="C28" s="105"/>
-      <c r="D28" s="105"/>
-      <c r="E28" s="105"/>
-      <c r="F28" s="105"/>
-      <c r="G28" s="105"/>
-      <c r="H28" s="105"/>
-      <c r="I28" s="105"/>
+      <c r="C28" s="107"/>
+      <c r="D28" s="107"/>
+      <c r="E28" s="107"/>
+      <c r="F28" s="107"/>
+      <c r="G28" s="107"/>
+      <c r="H28" s="107"/>
+      <c r="I28" s="107"/>
     </row>
     <row r="29" ht="14.35" customHeight="1">
-      <c r="A29" t="s" s="103">
+      <c r="A29" t="s" s="105">
         <v>62</v>
       </c>
-      <c r="B29" t="s" s="104">
+      <c r="B29" t="s" s="106">
         <v>63</v>
       </c>
-      <c r="C29" s="106">
+      <c r="C29" s="108">
         <v>2</v>
       </c>
-      <c r="D29" s="105"/>
-      <c r="E29" s="105"/>
-      <c r="F29" t="s" s="107">
+      <c r="D29" s="107"/>
+      <c r="E29" s="107"/>
+      <c r="F29" t="s" s="109">
         <v>210</v>
       </c>
-      <c r="G29" s="105"/>
-      <c r="H29" s="106">
+      <c r="G29" s="107"/>
+      <c r="H29" s="108">
         <v>127.63</v>
       </c>
-      <c r="I29" s="105"/>
+      <c r="I29" s="107"/>
     </row>
     <row r="30" ht="14.35" customHeight="1">
-      <c r="A30" t="s" s="103">
+      <c r="A30" t="s" s="105">
         <v>64</v>
       </c>
-      <c r="B30" t="s" s="104">
+      <c r="B30" t="s" s="106">
         <v>65</v>
       </c>
-      <c r="C30" s="106">
+      <c r="C30" s="108">
         <v>1.4</v>
       </c>
-      <c r="D30" s="106">
+      <c r="D30" s="108">
         <v>1.02</v>
       </c>
-      <c r="E30" s="106">
+      <c r="E30" s="108">
         <v>0.67</v>
       </c>
-      <c r="F30" t="s" s="107">
+      <c r="F30" t="s" s="109">
         <v>210</v>
       </c>
-      <c r="G30" t="s" s="107">
+      <c r="G30" t="s" s="109">
         <v>218</v>
       </c>
-      <c r="H30" s="105"/>
-      <c r="I30" s="105"/>
+      <c r="H30" s="107"/>
+      <c r="I30" s="107"/>
     </row>
     <row r="31" ht="14.35" customHeight="1">
-      <c r="A31" t="s" s="103">
+      <c r="A31" t="s" s="105">
         <v>66</v>
       </c>
-      <c r="B31" t="s" s="104">
+      <c r="B31" t="s" s="106">
         <v>67</v>
       </c>
-      <c r="C31" s="105"/>
-      <c r="D31" s="105"/>
-      <c r="E31" s="105"/>
-      <c r="F31" s="105"/>
-      <c r="G31" s="105"/>
-      <c r="H31" s="105"/>
-      <c r="I31" s="105"/>
+      <c r="C31" s="107"/>
+      <c r="D31" s="107"/>
+      <c r="E31" s="107"/>
+      <c r="F31" s="107"/>
+      <c r="G31" s="107"/>
+      <c r="H31" s="107"/>
+      <c r="I31" s="107"/>
     </row>
     <row r="32" ht="14.35" customHeight="1">
-      <c r="A32" t="s" s="103">
+      <c r="A32" t="s" s="105">
         <v>68</v>
       </c>
-      <c r="B32" t="s" s="104">
+      <c r="B32" t="s" s="106">
         <v>69</v>
       </c>
-      <c r="C32" s="105"/>
-      <c r="D32" s="105"/>
-      <c r="E32" s="105"/>
-      <c r="F32" s="105"/>
-      <c r="G32" s="105"/>
-      <c r="H32" s="105"/>
-      <c r="I32" s="105"/>
+      <c r="C32" s="107"/>
+      <c r="D32" s="107"/>
+      <c r="E32" s="107"/>
+      <c r="F32" s="107"/>
+      <c r="G32" s="107"/>
+      <c r="H32" s="107"/>
+      <c r="I32" s="107"/>
     </row>
     <row r="33" ht="14.35" customHeight="1">
-      <c r="A33" t="s" s="103">
+      <c r="A33" t="s" s="105">
         <v>70</v>
       </c>
-      <c r="B33" t="s" s="104">
+      <c r="B33" t="s" s="106">
         <v>71</v>
       </c>
-      <c r="C33" s="105"/>
-      <c r="D33" s="105"/>
-      <c r="E33" s="105"/>
-      <c r="F33" s="105"/>
-      <c r="G33" s="105"/>
-      <c r="H33" s="105"/>
-      <c r="I33" s="105"/>
+      <c r="C33" s="107"/>
+      <c r="D33" s="107"/>
+      <c r="E33" s="107"/>
+      <c r="F33" s="107"/>
+      <c r="G33" s="107"/>
+      <c r="H33" s="107"/>
+      <c r="I33" s="107"/>
     </row>
     <row r="34" ht="14.35" customHeight="1">
-      <c r="A34" t="s" s="103">
+      <c r="A34" t="s" s="105">
         <v>72</v>
       </c>
-      <c r="B34" t="s" s="104">
+      <c r="B34" t="s" s="106">
         <v>73</v>
       </c>
-      <c r="C34" s="105"/>
-      <c r="D34" s="105"/>
-      <c r="E34" s="105"/>
-      <c r="F34" s="105"/>
-      <c r="G34" s="105"/>
-      <c r="H34" s="105"/>
-      <c r="I34" s="105"/>
+      <c r="C34" s="107"/>
+      <c r="D34" s="107"/>
+      <c r="E34" s="107"/>
+      <c r="F34" s="107"/>
+      <c r="G34" s="107"/>
+      <c r="H34" s="107"/>
+      <c r="I34" s="107"/>
     </row>
     <row r="35" ht="14.35" customHeight="1">
-      <c r="A35" t="s" s="103">
+      <c r="A35" t="s" s="105">
         <v>74</v>
       </c>
-      <c r="B35" t="s" s="104">
+      <c r="B35" t="s" s="106">
         <v>75</v>
       </c>
-      <c r="C35" s="105"/>
-      <c r="D35" s="105"/>
-      <c r="E35" s="105"/>
-      <c r="F35" s="105"/>
-      <c r="G35" s="105"/>
-      <c r="H35" s="105"/>
-      <c r="I35" s="105"/>
+      <c r="C35" s="107"/>
+      <c r="D35" s="107"/>
+      <c r="E35" s="107"/>
+      <c r="F35" s="107"/>
+      <c r="G35" s="107"/>
+      <c r="H35" s="107"/>
+      <c r="I35" s="107"/>
     </row>
     <row r="36" ht="14.35" customHeight="1">
-      <c r="A36" t="s" s="103">
+      <c r="A36" t="s" s="105">
         <v>76</v>
       </c>
-      <c r="B36" t="s" s="104">
+      <c r="B36" t="s" s="106">
         <v>77</v>
       </c>
-      <c r="C36" s="105"/>
-      <c r="D36" s="105"/>
-      <c r="E36" s="105"/>
-      <c r="F36" s="105"/>
-      <c r="G36" s="105"/>
-      <c r="H36" s="105"/>
-      <c r="I36" s="105"/>
+      <c r="C36" s="107"/>
+      <c r="D36" s="107"/>
+      <c r="E36" s="107"/>
+      <c r="F36" s="107"/>
+      <c r="G36" s="107"/>
+      <c r="H36" s="107"/>
+      <c r="I36" s="107"/>
     </row>
     <row r="37" ht="14.35" customHeight="1">
-      <c r="A37" t="s" s="103">
+      <c r="A37" t="s" s="105">
         <v>78</v>
       </c>
-      <c r="B37" t="s" s="104">
+      <c r="B37" t="s" s="106">
         <v>79</v>
       </c>
-      <c r="C37" s="105"/>
-      <c r="D37" s="105"/>
-      <c r="E37" s="105"/>
-      <c r="F37" s="105"/>
-      <c r="G37" s="105"/>
-      <c r="H37" s="105"/>
-      <c r="I37" s="105"/>
+      <c r="C37" s="107"/>
+      <c r="D37" s="107"/>
+      <c r="E37" s="107"/>
+      <c r="F37" s="107"/>
+      <c r="G37" s="107"/>
+      <c r="H37" s="107"/>
+      <c r="I37" s="107"/>
     </row>
     <row r="38" ht="14.35" customHeight="1">
-      <c r="A38" t="s" s="103">
+      <c r="A38" t="s" s="105">
         <v>80</v>
       </c>
-      <c r="B38" t="s" s="104">
+      <c r="B38" t="s" s="106">
         <v>81</v>
       </c>
-      <c r="C38" s="105"/>
-      <c r="D38" s="105"/>
-      <c r="E38" s="105"/>
-      <c r="F38" s="105"/>
-      <c r="G38" s="105"/>
-      <c r="H38" s="105"/>
-      <c r="I38" s="105"/>
+      <c r="C38" s="107"/>
+      <c r="D38" s="107"/>
+      <c r="E38" s="107"/>
+      <c r="F38" s="107"/>
+      <c r="G38" s="107"/>
+      <c r="H38" s="107"/>
+      <c r="I38" s="107"/>
     </row>
     <row r="39" ht="14.35" customHeight="1">
-      <c r="A39" t="s" s="103">
+      <c r="A39" t="s" s="105">
         <v>82</v>
       </c>
-      <c r="B39" t="s" s="104">
+      <c r="B39" t="s" s="106">
         <v>83</v>
       </c>
-      <c r="C39" s="105"/>
-      <c r="D39" s="105"/>
-      <c r="E39" s="105"/>
-      <c r="F39" s="105"/>
-      <c r="G39" s="105"/>
-      <c r="H39" s="105"/>
-      <c r="I39" s="105"/>
+      <c r="C39" s="107"/>
+      <c r="D39" s="107"/>
+      <c r="E39" s="107"/>
+      <c r="F39" s="107"/>
+      <c r="G39" s="107"/>
+      <c r="H39" s="107"/>
+      <c r="I39" s="107"/>
     </row>
     <row r="40" ht="14.35" customHeight="1">
-      <c r="A40" t="s" s="103">
+      <c r="A40" t="s" s="105">
         <v>84</v>
       </c>
-      <c r="B40" t="s" s="104">
+      <c r="B40" t="s" s="106">
         <v>85</v>
       </c>
-      <c r="C40" s="105"/>
-      <c r="D40" s="105"/>
-      <c r="E40" s="105"/>
-      <c r="F40" s="105"/>
-      <c r="G40" s="105"/>
-      <c r="H40" s="105"/>
-      <c r="I40" s="105"/>
+      <c r="C40" s="107"/>
+      <c r="D40" s="107"/>
+      <c r="E40" s="107"/>
+      <c r="F40" s="107"/>
+      <c r="G40" s="107"/>
+      <c r="H40" s="107"/>
+      <c r="I40" s="107"/>
     </row>
     <row r="41" ht="15.95" customHeight="1">
-      <c r="A41" t="s" s="103">
+      <c r="A41" t="s" s="105">
         <v>86</v>
       </c>
-      <c r="B41" t="s" s="104">
+      <c r="B41" t="s" s="106">
         <v>87</v>
       </c>
-      <c r="C41" s="106">
+      <c r="C41" s="108">
         <v>352</v>
       </c>
-      <c r="D41" s="106">
+      <c r="D41" s="108">
         <v>381</v>
       </c>
-      <c r="E41" s="106">
+      <c r="E41" s="108">
         <v>334</v>
       </c>
-      <c r="F41" t="s" s="107">
+      <c r="F41" t="s" s="109">
         <v>204</v>
       </c>
-      <c r="G41" t="s" s="116">
+      <c r="G41" t="s" s="118">
         <v>219</v>
       </c>
-      <c r="H41" s="105"/>
-      <c r="I41" t="s" s="107">
+      <c r="H41" s="107"/>
+      <c r="I41" t="s" s="109">
         <v>220</v>
       </c>
     </row>
     <row r="42" ht="14.35" customHeight="1">
-      <c r="A42" t="s" s="103">
+      <c r="A42" t="s" s="105">
         <v>88</v>
       </c>
-      <c r="B42" t="s" s="104">
+      <c r="B42" t="s" s="106">
         <v>89</v>
       </c>
-      <c r="C42" s="105"/>
-      <c r="D42" s="105"/>
-      <c r="E42" s="105"/>
-      <c r="F42" s="105"/>
-      <c r="G42" s="105"/>
-      <c r="H42" s="105"/>
-      <c r="I42" s="105"/>
+      <c r="C42" s="107"/>
+      <c r="D42" s="107"/>
+      <c r="E42" s="107"/>
+      <c r="F42" s="107"/>
+      <c r="G42" s="107"/>
+      <c r="H42" s="107"/>
+      <c r="I42" s="107"/>
     </row>
     <row r="43" ht="14.35" customHeight="1">
-      <c r="A43" t="s" s="103">
+      <c r="A43" t="s" s="105">
         <v>90</v>
       </c>
-      <c r="B43" t="s" s="104">
+      <c r="B43" t="s" s="106">
         <v>91</v>
       </c>
-      <c r="C43" s="105"/>
-      <c r="D43" s="105"/>
-      <c r="E43" s="105"/>
-      <c r="F43" s="105"/>
-      <c r="G43" s="105"/>
-      <c r="H43" s="105"/>
-      <c r="I43" s="105"/>
+      <c r="C43" s="107"/>
+      <c r="D43" s="107"/>
+      <c r="E43" s="107"/>
+      <c r="F43" s="107"/>
+      <c r="G43" s="107"/>
+      <c r="H43" s="107"/>
+      <c r="I43" s="107"/>
     </row>
     <row r="44" ht="14.35" customHeight="1">
-      <c r="A44" t="s" s="103">
+      <c r="A44" t="s" s="105">
         <v>92</v>
       </c>
-      <c r="B44" t="s" s="104">
+      <c r="B44" t="s" s="106">
         <v>93</v>
       </c>
-      <c r="C44" s="105"/>
-      <c r="D44" s="105"/>
-      <c r="E44" s="105"/>
-      <c r="F44" s="105"/>
-      <c r="G44" s="105"/>
-      <c r="H44" s="105"/>
-      <c r="I44" s="105"/>
+      <c r="C44" s="107"/>
+      <c r="D44" s="107"/>
+      <c r="E44" s="107"/>
+      <c r="F44" s="107"/>
+      <c r="G44" s="107"/>
+      <c r="H44" s="107"/>
+      <c r="I44" s="107"/>
     </row>
     <row r="45" ht="14.35" customHeight="1">
-      <c r="A45" t="s" s="103">
+      <c r="A45" t="s" s="105">
         <v>94</v>
       </c>
-      <c r="B45" t="s" s="104">
+      <c r="B45" t="s" s="106">
         <v>95</v>
       </c>
-      <c r="C45" s="105"/>
-      <c r="D45" s="105"/>
-      <c r="E45" s="105"/>
-      <c r="F45" s="105"/>
-      <c r="G45" s="105"/>
-      <c r="H45" s="105"/>
-      <c r="I45" s="105"/>
+      <c r="C45" s="108">
+        <v>34.1</v>
+      </c>
+      <c r="D45" s="107"/>
+      <c r="E45" s="108">
+        <v>25.1</v>
+      </c>
+      <c r="F45" t="s" s="109">
+        <v>206</v>
+      </c>
+      <c r="G45" s="115">
+        <v>64.34</v>
+      </c>
+      <c r="H45" s="115">
+        <v>69.27</v>
+      </c>
+      <c r="I45" s="107"/>
     </row>
     <row r="46" ht="14.35" customHeight="1">
-      <c r="A46" t="s" s="103">
+      <c r="A46" t="s" s="105">
         <v>96</v>
       </c>
-      <c r="B46" t="s" s="104">
+      <c r="B46" t="s" s="106">
         <v>97</v>
       </c>
-      <c r="C46" s="105"/>
-      <c r="D46" s="105"/>
-      <c r="E46" s="105"/>
-      <c r="F46" s="105"/>
-      <c r="G46" s="105"/>
-      <c r="H46" s="105"/>
-      <c r="I46" s="105"/>
+      <c r="C46" s="107"/>
+      <c r="D46" s="107"/>
+      <c r="E46" s="107"/>
+      <c r="F46" s="107"/>
+      <c r="G46" s="107"/>
+      <c r="H46" s="107"/>
+      <c r="I46" s="107"/>
     </row>
     <row r="47" ht="14.35" customHeight="1">
-      <c r="A47" t="s" s="103">
+      <c r="A47" t="s" s="105">
         <v>98</v>
       </c>
-      <c r="B47" t="s" s="104">
+      <c r="B47" t="s" s="106">
         <v>99</v>
       </c>
-      <c r="C47" s="105"/>
-      <c r="D47" s="105"/>
-      <c r="E47" s="105"/>
-      <c r="F47" s="105"/>
-      <c r="G47" s="105"/>
-      <c r="H47" s="105"/>
-      <c r="I47" s="105"/>
+      <c r="C47" s="107"/>
+      <c r="D47" s="107"/>
+      <c r="E47" s="107"/>
+      <c r="F47" s="107"/>
+      <c r="G47" s="107"/>
+      <c r="H47" s="107"/>
+      <c r="I47" s="107"/>
     </row>
     <row r="48" ht="14.35" customHeight="1">
-      <c r="A48" t="s" s="103">
+      <c r="A48" t="s" s="105">
         <v>100</v>
       </c>
-      <c r="B48" t="s" s="104">
+      <c r="B48" t="s" s="106">
         <v>101</v>
       </c>
-      <c r="C48" s="105"/>
-      <c r="D48" s="105"/>
-      <c r="E48" s="105"/>
-      <c r="F48" s="105"/>
-      <c r="G48" s="105"/>
-      <c r="H48" s="105"/>
-      <c r="I48" s="105"/>
+      <c r="C48" s="107"/>
+      <c r="D48" s="107"/>
+      <c r="E48" s="107"/>
+      <c r="F48" s="107"/>
+      <c r="G48" s="107"/>
+      <c r="H48" s="107"/>
+      <c r="I48" s="107"/>
     </row>
     <row r="49" ht="14.35" customHeight="1">
-      <c r="A49" t="s" s="103">
+      <c r="A49" t="s" s="105">
         <v>102</v>
       </c>
-      <c r="B49" t="s" s="104">
+      <c r="B49" t="s" s="106">
         <v>103</v>
       </c>
-      <c r="C49" s="105"/>
-      <c r="D49" s="105"/>
-      <c r="E49" s="105"/>
-      <c r="F49" s="105"/>
-      <c r="G49" s="105"/>
-      <c r="H49" s="105"/>
-      <c r="I49" s="105"/>
+      <c r="C49" s="107"/>
+      <c r="D49" s="107"/>
+      <c r="E49" s="107"/>
+      <c r="F49" s="107"/>
+      <c r="G49" s="107"/>
+      <c r="H49" s="107"/>
+      <c r="I49" s="107"/>
     </row>
     <row r="50" ht="14.35" customHeight="1">
-      <c r="A50" t="s" s="103">
+      <c r="A50" t="s" s="105">
         <v>104</v>
       </c>
-      <c r="B50" t="s" s="104">
+      <c r="B50" t="s" s="106">
         <v>105</v>
       </c>
-      <c r="C50" s="105"/>
-      <c r="D50" s="105"/>
-      <c r="E50" s="105"/>
-      <c r="F50" s="105"/>
-      <c r="G50" s="105"/>
-      <c r="H50" s="105"/>
-      <c r="I50" s="105"/>
+      <c r="C50" s="107"/>
+      <c r="D50" s="107"/>
+      <c r="E50" s="107"/>
+      <c r="F50" s="107"/>
+      <c r="G50" s="107"/>
+      <c r="H50" s="107"/>
+      <c r="I50" s="107"/>
     </row>
     <row r="51" ht="14.35" customHeight="1">
-      <c r="A51" t="s" s="103">
+      <c r="A51" t="s" s="105">
         <v>106</v>
       </c>
-      <c r="B51" t="s" s="104">
+      <c r="B51" t="s" s="106">
         <v>107</v>
       </c>
-      <c r="C51" s="105"/>
-      <c r="D51" s="105"/>
-      <c r="E51" s="105"/>
-      <c r="F51" s="105"/>
-      <c r="G51" s="105"/>
-      <c r="H51" s="105"/>
-      <c r="I51" s="105"/>
+      <c r="C51" s="107"/>
+      <c r="D51" s="107"/>
+      <c r="E51" s="107"/>
+      <c r="F51" s="107"/>
+      <c r="G51" s="107"/>
+      <c r="H51" s="107"/>
+      <c r="I51" s="107"/>
     </row>
     <row r="52" ht="14.35" customHeight="1">
-      <c r="A52" t="s" s="103">
+      <c r="A52" t="s" s="105">
         <v>108</v>
       </c>
-      <c r="B52" t="s" s="104">
+      <c r="B52" t="s" s="106">
         <v>109</v>
       </c>
-      <c r="C52" s="106">
+      <c r="C52" s="108">
         <v>26</v>
       </c>
-      <c r="D52" s="106">
+      <c r="D52" s="108">
         <v>22</v>
       </c>
-      <c r="E52" s="106">
+      <c r="E52" s="108">
         <v>12</v>
       </c>
-      <c r="F52" t="s" s="107">
+      <c r="F52" t="s" s="109">
         <v>206</v>
       </c>
-      <c r="G52" s="105"/>
-      <c r="H52" s="105"/>
-      <c r="I52" t="s" s="107">
+      <c r="G52" s="107"/>
+      <c r="H52" s="107"/>
+      <c r="I52" t="s" s="109">
         <v>221</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:I1"/>
+  </mergeCells>
+  <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>
+  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
+  <headerFooter>
+    <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A2:B52"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1">
+      <pane topLeftCell="B3" xSplit="1" ySplit="2" activePane="bottomRight" state="frozen"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="14.75" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col min="1" max="1" width="16.3516" style="121" customWidth="1"/>
+    <col min="2" max="2" width="16.3516" style="121" customWidth="1"/>
+    <col min="3" max="256" width="16.3516" style="121" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="16" customHeight="1">
+      <c r="A1" t="s" s="122">
+        <v>197</v>
+      </c>
+      <c r="B1" s="122"/>
+    </row>
+    <row r="2" ht="19.55" customHeight="1">
+      <c r="A2" t="s" s="123">
+        <v>222</v>
+      </c>
+      <c r="B2" t="s" s="124">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" ht="19.55" customHeight="1">
+      <c r="A3" t="s" s="125">
+        <v>223</v>
+      </c>
+      <c r="B3" t="s" s="126">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" ht="19.35" customHeight="1">
+      <c r="A4" t="s" s="127">
+        <v>223</v>
+      </c>
+      <c r="B4" t="s" s="128">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" ht="19.35" customHeight="1">
+      <c r="A5" t="s" s="127">
+        <v>223</v>
+      </c>
+      <c r="B5" t="s" s="128">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" ht="19.35" customHeight="1">
+      <c r="A6" s="129"/>
+      <c r="B6" t="s" s="128">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" ht="19.35" customHeight="1">
+      <c r="A7" s="129"/>
+      <c r="B7" t="s" s="128">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" ht="19.35" customHeight="1">
+      <c r="A8" t="s" s="127">
+        <v>223</v>
+      </c>
+      <c r="B8" t="s" s="128">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" ht="19.35" customHeight="1">
+      <c r="A9" t="s" s="127">
+        <v>223</v>
+      </c>
+      <c r="B9" t="s" s="128">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" ht="19.35" customHeight="1">
+      <c r="A10" t="s" s="127">
+        <v>223</v>
+      </c>
+      <c r="B10" t="s" s="128">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="11" ht="19.35" customHeight="1">
+      <c r="A11" s="129"/>
+      <c r="B11" t="s" s="128">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="12" ht="19.35" customHeight="1">
+      <c r="A12" s="129"/>
+      <c r="B12" t="s" s="128">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="13" ht="19.35" customHeight="1">
+      <c r="A13" s="129"/>
+      <c r="B13" t="s" s="128">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="14" ht="19.35" customHeight="1">
+      <c r="A14" s="130"/>
+      <c r="B14" t="s" s="128">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="15" ht="19.35" customHeight="1">
+      <c r="A15" t="s" s="127">
+        <v>223</v>
+      </c>
+      <c r="B15" t="s" s="128">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="16" ht="19.35" customHeight="1">
+      <c r="A16" t="s" s="127">
+        <v>223</v>
+      </c>
+      <c r="B16" t="s" s="128">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="17" ht="19.35" customHeight="1">
+      <c r="A17" s="130"/>
+      <c r="B17" t="s" s="128">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="18" ht="19.35" customHeight="1">
+      <c r="A18" s="130"/>
+      <c r="B18" t="s" s="128">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="19" ht="19.35" customHeight="1">
+      <c r="A19" s="130"/>
+      <c r="B19" t="s" s="128">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="20" ht="19.35" customHeight="1">
+      <c r="A20" t="s" s="127">
+        <v>223</v>
+      </c>
+      <c r="B20" t="s" s="128">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="21" ht="19.35" customHeight="1">
+      <c r="A21" t="s" s="127">
+        <v>223</v>
+      </c>
+      <c r="B21" t="s" s="128">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="22" ht="19.35" customHeight="1">
+      <c r="A22" t="s" s="127">
+        <v>223</v>
+      </c>
+      <c r="B22" t="s" s="128">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="23" ht="19.35" customHeight="1">
+      <c r="A23" s="129"/>
+      <c r="B23" t="s" s="128">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="24" ht="19.35" customHeight="1">
+      <c r="A24" s="129"/>
+      <c r="B24" t="s" s="128">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="25" ht="19.35" customHeight="1">
+      <c r="A25" s="129"/>
+      <c r="B25" t="s" s="128">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="26" ht="19.35" customHeight="1">
+      <c r="A26" s="129"/>
+      <c r="B26" t="s" s="128">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="27" ht="19.35" customHeight="1">
+      <c r="A27" t="s" s="127">
+        <v>223</v>
+      </c>
+      <c r="B27" t="s" s="128">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="28" ht="19.35" customHeight="1">
+      <c r="A28" s="129"/>
+      <c r="B28" t="s" s="128">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="29" ht="19.35" customHeight="1">
+      <c r="A29" t="s" s="127">
+        <v>223</v>
+      </c>
+      <c r="B29" t="s" s="128">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="30" ht="19.35" customHeight="1">
+      <c r="A30" s="129"/>
+      <c r="B30" t="s" s="128">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="31" ht="19.35" customHeight="1">
+      <c r="A31" s="129"/>
+      <c r="B31" t="s" s="128">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="32" ht="19.35" customHeight="1">
+      <c r="A32" s="129"/>
+      <c r="B32" t="s" s="128">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="33" ht="19.35" customHeight="1">
+      <c r="A33" s="130"/>
+      <c r="B33" t="s" s="128">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="34" ht="19.35" customHeight="1">
+      <c r="A34" s="129"/>
+      <c r="B34" t="s" s="128">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="35" ht="19.35" customHeight="1">
+      <c r="A35" t="s" s="127">
+        <v>223</v>
+      </c>
+      <c r="B35" t="s" s="128">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="36" ht="19.35" customHeight="1">
+      <c r="A36" t="s" s="127">
+        <v>223</v>
+      </c>
+      <c r="B36" t="s" s="128">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="37" ht="19.35" customHeight="1">
+      <c r="A37" s="129"/>
+      <c r="B37" t="s" s="128">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="38" ht="19.35" customHeight="1">
+      <c r="A38" t="s" s="127">
+        <v>223</v>
+      </c>
+      <c r="B38" t="s" s="128">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="39" ht="19.35" customHeight="1">
+      <c r="A39" s="129"/>
+      <c r="B39" t="s" s="128">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="40" ht="19.35" customHeight="1">
+      <c r="A40" s="129"/>
+      <c r="B40" t="s" s="128">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="41" ht="19.35" customHeight="1">
+      <c r="A41" t="s" s="127">
+        <v>223</v>
+      </c>
+      <c r="B41" t="s" s="128">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="42" ht="19.35" customHeight="1">
+      <c r="A42" s="129"/>
+      <c r="B42" t="s" s="128">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="43" ht="19.35" customHeight="1">
+      <c r="A43" s="129"/>
+      <c r="B43" t="s" s="128">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="44" ht="19.35" customHeight="1">
+      <c r="A44" s="129"/>
+      <c r="B44" t="s" s="128">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="45" ht="19.35" customHeight="1">
+      <c r="A45" t="s" s="127">
+        <v>223</v>
+      </c>
+      <c r="B45" t="s" s="128">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="46" ht="19.35" customHeight="1">
+      <c r="A46" s="130"/>
+      <c r="B46" t="s" s="128">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="47" ht="19.35" customHeight="1">
+      <c r="A47" t="s" s="127">
+        <v>223</v>
+      </c>
+      <c r="B47" t="s" s="128">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="48" ht="19.35" customHeight="1">
+      <c r="A48" s="129"/>
+      <c r="B48" t="s" s="128">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="49" ht="19.35" customHeight="1">
+      <c r="A49" s="130"/>
+      <c r="B49" t="s" s="128">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="50" ht="19.35" customHeight="1">
+      <c r="A50" t="s" s="127">
+        <v>223</v>
+      </c>
+      <c r="B50" t="s" s="128">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="51" ht="19.35" customHeight="1">
+      <c r="A51" s="130"/>
+      <c r="B51" t="s" s="128">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="52" ht="19.35" customHeight="1">
+      <c r="A52" t="s" s="127">
+        <v>223</v>
+      </c>
+      <c r="B52" t="s" s="128">
+        <v>109</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:B1"/>
   </mergeCells>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>
   <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>

</xml_diff>